<commit_message>
Issue #27 Renamed Publication to Reference, introduced type OntologyTerm. Replaced "publications" to "references" in all test models.
</commit_message>
<xml_diff>
--- a/test/excel/Keast_Flatmap_neurolatorNeuron2.xlsx
+++ b/test/excel/Keast_Flatmap_neurolatorNeuron2.xlsx
@@ -11,14 +11,14 @@
     <sheet state="visible" name="nodes" sheetId="6" r:id="rId9"/>
     <sheet state="visible" name="neurons" sheetId="7" r:id="rId10"/>
     <sheet state="visible" name="groups" sheetId="8" r:id="rId11"/>
-    <sheet state="visible" name="publications" sheetId="9" r:id="rId12"/>
+    <sheet state="visible" name="references" sheetId="9" r:id="rId12"/>
     <sheet state="visible" name="localConventions" sheetId="10" r:id="rId13"/>
   </sheets>
   <definedNames/>
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId14" roundtripDataSignature="AMtx7mjJ0E35peh9dp4cCn15t30XOq0sdQ=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId14" roundtripDataSignature="AMtx7mhkddWutpixBXx1M4/nC8P+50n4QA=="/>
     </ext>
   </extLst>
 </workbook>
@@ -133,7 +133,7 @@
   </commentList>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7mioLSU6sDIfqt5Cv2yOX+9s0Zqq9w=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7mhf5vhBr9YH9HwzqnYoeyl9g7+bAw=="/>
     </ext>
   </extLst>
 </comments>
@@ -163,7 +163,7 @@
   </commentList>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7miRXmCpQJk5+aZGYiTk1KAl48YqpA=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7miOmA1jsfzFKailuQPDMkmoaaJn/Q=="/>
     </ext>
   </extLst>
 </comments>
@@ -187,7 +187,7 @@
   </commentList>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7miUyV79QA9KuNn/wvoSUi8UejUCpQ=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7mhctYkkG+oEgCwNF2vzwO72MN3oPQ=="/>
     </ext>
   </extLst>
 </comments>
@@ -220,14 +220,14 @@
   </commentList>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7mjKtv6Q3FyvJtTLXeRVmusOefgsVg=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7mgu/fThSRKvU4TvvJ+L0QCYGpjD2g=="/>
     </ext>
   </extLst>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="706" uniqueCount="562">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="706" uniqueCount="563">
   <si>
     <t>id</t>
   </si>
@@ -491,6 +491,9 @@
     <t>NLX:154731</t>
   </si>
   <si>
+    <t>229bag2</t>
+  </si>
+  <si>
     <t>Segment of neuron  (kblad)</t>
   </si>
   <si>
@@ -755,9 +758,6 @@
     <t>ILX:0777093</t>
   </si>
   <si>
-    <t>k</t>
-  </si>
-  <si>
     <t>K78</t>
   </si>
   <si>
@@ -1728,6 +1728,9 @@
   </si>
   <si>
     <t>groups</t>
+  </si>
+  <si>
+    <t>references</t>
   </si>
   <si>
     <t>neuron-2</t>
@@ -2081,7 +2084,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="74">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -2146,6 +2149,9 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" vertical="bottom"/>
@@ -2223,9 +2229,6 @@
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -2258,14 +2261,11 @@
     <xf borderId="0" fillId="6" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="6" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="6" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
+      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
@@ -3575,106 +3575,106 @@
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="7" t="s">
-        <v>538</v>
-      </c>
-      <c r="B2" s="73" t="s">
         <v>539</v>
+      </c>
+      <c r="B2" s="72" t="s">
+        <v>540</v>
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="7" t="s">
-        <v>540</v>
-      </c>
-      <c r="B3" s="74" t="s">
         <v>541</v>
+      </c>
+      <c r="B3" s="73" t="s">
+        <v>542</v>
       </c>
     </row>
     <row r="4" ht="15.75" customHeight="1">
       <c r="A4" s="7" t="s">
-        <v>542</v>
-      </c>
-      <c r="B4" s="74" t="s">
         <v>543</v>
+      </c>
+      <c r="B4" s="73" t="s">
+        <v>544</v>
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="7" t="s">
-        <v>544</v>
-      </c>
-      <c r="B5" s="74" t="s">
         <v>545</v>
+      </c>
+      <c r="B5" s="73" t="s">
+        <v>546</v>
       </c>
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="7" t="s">
-        <v>546</v>
-      </c>
-      <c r="B6" s="74" t="s">
         <v>547</v>
+      </c>
+      <c r="B6" s="73" t="s">
+        <v>548</v>
       </c>
     </row>
     <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="7" t="s">
-        <v>548</v>
-      </c>
-      <c r="B7" s="74" t="s">
         <v>549</v>
+      </c>
+      <c r="B7" s="73" t="s">
+        <v>550</v>
       </c>
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="7" t="s">
-        <v>550</v>
-      </c>
-      <c r="B8" s="74" t="s">
         <v>551</v>
+      </c>
+      <c r="B8" s="73" t="s">
+        <v>552</v>
       </c>
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="7" t="s">
-        <v>552</v>
-      </c>
-      <c r="B9" s="74" t="s">
         <v>553</v>
+      </c>
+      <c r="B9" s="73" t="s">
+        <v>554</v>
       </c>
     </row>
     <row r="10" ht="15.75" customHeight="1">
       <c r="A10" s="7" t="s">
-        <v>554</v>
-      </c>
-      <c r="B10" s="74" t="s">
         <v>555</v>
+      </c>
+      <c r="B10" s="73" t="s">
+        <v>556</v>
       </c>
     </row>
     <row r="11" ht="15.75" customHeight="1">
       <c r="A11" s="7" t="s">
-        <v>556</v>
-      </c>
-      <c r="B11" s="74" t="s">
         <v>557</v>
+      </c>
+      <c r="B11" s="73" t="s">
+        <v>558</v>
       </c>
     </row>
     <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="2" t="s">
-        <v>558</v>
-      </c>
-      <c r="B12" s="70" t="s">
         <v>559</v>
+      </c>
+      <c r="B12" s="69" t="s">
+        <v>560</v>
       </c>
     </row>
     <row r="13" ht="15.75" customHeight="1">
       <c r="A13" s="2" t="s">
-        <v>560</v>
-      </c>
-      <c r="B13" s="70" t="s">
         <v>561</v>
+      </c>
+      <c r="B13" s="69" t="s">
+        <v>562</v>
       </c>
     </row>
     <row r="14" ht="15.75" customHeight="1"/>
@@ -4698,7 +4698,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="14.57"/>
+    <col customWidth="1" min="1" max="1" width="29.71"/>
     <col customWidth="1" min="2" max="2" width="60.14"/>
     <col customWidth="1" min="3" max="3" width="18.57"/>
     <col customWidth="1" min="4" max="4" width="11.29"/>
@@ -5266,8 +5266,11 @@
       <c r="Q17" s="7"/>
     </row>
     <row r="18" ht="15.75" customHeight="1">
-      <c r="A18" s="7" t="s">
+      <c r="A18" s="23" t="s">
         <v>87</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>88</v>
       </c>
       <c r="C18" s="8" t="s">
         <v>83</v>
@@ -5277,12 +5280,12 @@
         <v>1</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="G18" s="7"/>
       <c r="H18" s="7"/>
       <c r="I18" s="7"/>
-      <c r="J18" s="23">
+      <c r="J18" s="24">
         <v>229.0</v>
       </c>
       <c r="K18" s="7"/>
@@ -5295,7 +5298,7 @@
     </row>
     <row r="19" ht="15.75" customHeight="1">
       <c r="A19" s="11" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B19" s="7" t="s">
         <v>82</v>
@@ -5308,12 +5311,12 @@
         <v>1</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="G19" s="7"/>
       <c r="H19" s="7"/>
       <c r="I19" s="7"/>
-      <c r="J19" s="23">
+      <c r="J19" s="24">
         <v>229.0</v>
       </c>
       <c r="K19" s="7"/>
@@ -5329,7 +5332,7 @@
         <v>64</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C20" s="20" t="s">
         <v>86</v>
@@ -5340,7 +5343,7 @@
       <c r="G20" s="7"/>
       <c r="H20" s="7"/>
       <c r="I20" s="7"/>
-      <c r="J20" s="23">
+      <c r="J20" s="24">
         <v>229.0</v>
       </c>
       <c r="K20" s="7"/>
@@ -5358,7 +5361,7 @@
         <v>39</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C21" s="20" t="s">
         <v>86</v>
@@ -5369,7 +5372,7 @@
       <c r="G21" s="7"/>
       <c r="H21" s="7"/>
       <c r="I21" s="7"/>
-      <c r="J21" s="23">
+      <c r="J21" s="24">
         <v>229.0</v>
       </c>
       <c r="K21" s="7"/>
@@ -5387,7 +5390,7 @@
         <v>43</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C22" s="20" t="s">
         <v>86</v>
@@ -5398,7 +5401,7 @@
       <c r="G22" s="7"/>
       <c r="H22" s="7"/>
       <c r="I22" s="7"/>
-      <c r="J22" s="23">
+      <c r="J22" s="24">
         <v>229.0</v>
       </c>
       <c r="K22" s="7"/>
@@ -5416,7 +5419,7 @@
         <v>52</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C23" s="20" t="s">
         <v>86</v>
@@ -5427,7 +5430,7 @@
       <c r="G23" s="7"/>
       <c r="H23" s="7"/>
       <c r="I23" s="7"/>
-      <c r="J23" s="23">
+      <c r="J23" s="24">
         <v>229.0</v>
       </c>
       <c r="K23" s="7"/>
@@ -5445,7 +5448,7 @@
         <v>56</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C24" s="20" t="s">
         <v>86</v>
@@ -5456,7 +5459,7 @@
       <c r="G24" s="7"/>
       <c r="H24" s="7"/>
       <c r="I24" s="7"/>
-      <c r="J24" s="23">
+      <c r="J24" s="24">
         <v>229.0</v>
       </c>
       <c r="K24" s="7"/>
@@ -5474,7 +5477,7 @@
         <v>60</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C25" s="20" t="s">
         <v>86</v>
@@ -5485,7 +5488,7 @@
       <c r="G25" s="7"/>
       <c r="H25" s="7"/>
       <c r="I25" s="7"/>
-      <c r="J25" s="23">
+      <c r="J25" s="24">
         <v>229.0</v>
       </c>
       <c r="K25" s="7"/>
@@ -5503,7 +5506,7 @@
         <v>71</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C26" s="20" t="s">
         <v>86</v>
@@ -5514,7 +5517,7 @@
       <c r="G26" s="7"/>
       <c r="H26" s="7"/>
       <c r="I26" s="7"/>
-      <c r="J26" s="23">
+      <c r="J26" s="24">
         <v>229.0</v>
       </c>
       <c r="K26" s="7"/>
@@ -5529,13 +5532,13 @@
     </row>
     <row r="27" ht="15.75" customHeight="1">
       <c r="A27" s="11" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D27" s="7"/>
       <c r="E27" s="7"/>
@@ -5554,13 +5557,13 @@
     </row>
     <row r="28" ht="15.75" customHeight="1">
       <c r="A28" s="11" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D28" s="7"/>
       <c r="E28" s="7"/>
@@ -5579,13 +5582,13 @@
     </row>
     <row r="29" ht="15.75" customHeight="1">
       <c r="A29" s="11" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D29" s="7"/>
       <c r="E29" s="7"/>
@@ -5597,7 +5600,7 @@
       <c r="K29" s="7"/>
       <c r="L29" s="11"/>
       <c r="M29" s="11" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="N29" s="11" t="s">
         <v>35</v>
@@ -5608,13 +5611,13 @@
     </row>
     <row r="30" ht="15.75" customHeight="1">
       <c r="A30" s="11" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D30" s="7"/>
       <c r="E30" s="7"/>
@@ -5626,7 +5629,7 @@
       <c r="K30" s="7"/>
       <c r="L30" s="11"/>
       <c r="M30" s="11" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="N30" s="11" t="s">
         <v>35</v>
@@ -5637,13 +5640,13 @@
     </row>
     <row r="31" ht="15.75" customHeight="1">
       <c r="A31" s="11" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D31" s="7"/>
       <c r="E31" s="7"/>
@@ -5662,13 +5665,13 @@
     </row>
     <row r="32" ht="15.75" customHeight="1">
       <c r="A32" s="11" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D32" s="7"/>
       <c r="E32" s="7"/>
@@ -5687,13 +5690,13 @@
     </row>
     <row r="33" ht="15.75" customHeight="1">
       <c r="A33" s="11" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D33" s="7"/>
       <c r="E33" s="7"/>
@@ -5712,13 +5715,13 @@
     </row>
     <row r="34" ht="15.75" customHeight="1">
       <c r="A34" s="11" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D34" s="7"/>
       <c r="E34" s="18"/>
@@ -5730,10 +5733,10 @@
       <c r="K34" s="7"/>
       <c r="L34" s="7"/>
       <c r="M34" s="7" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="N34" s="11" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="O34" s="7"/>
       <c r="P34" s="7"/>
@@ -5741,13 +5744,13 @@
     </row>
     <row r="35" ht="15.75" customHeight="1">
       <c r="A35" s="11" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D35" s="7"/>
       <c r="E35" s="18"/>
@@ -5759,10 +5762,10 @@
       <c r="K35" s="7"/>
       <c r="L35" s="7"/>
       <c r="M35" s="7" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="N35" s="11" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="O35" s="7"/>
       <c r="P35" s="7"/>
@@ -5770,13 +5773,13 @@
     </row>
     <row r="36" ht="15.75" customHeight="1">
       <c r="A36" s="11" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D36" s="7"/>
       <c r="E36" s="7"/>
@@ -5795,13 +5798,13 @@
     </row>
     <row r="37" ht="15.75" customHeight="1">
       <c r="A37" s="11" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D37" s="7"/>
       <c r="E37" s="7"/>
@@ -5820,13 +5823,13 @@
     </row>
     <row r="38" ht="15.75" customHeight="1">
       <c r="A38" s="11" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D38" s="7"/>
       <c r="E38" s="7"/>
@@ -5845,13 +5848,13 @@
     </row>
     <row r="39" ht="15.75" customHeight="1">
       <c r="A39" s="11" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D39" s="7"/>
       <c r="E39" s="7"/>
@@ -5870,13 +5873,13 @@
     </row>
     <row r="40" ht="15.75" customHeight="1">
       <c r="A40" s="11" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C40" s="7" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D40" s="7"/>
       <c r="E40" s="7"/>
@@ -5895,13 +5898,13 @@
     </row>
     <row r="41" ht="15.75" customHeight="1">
       <c r="A41" s="11" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D41" s="7"/>
       <c r="E41" s="7"/>
@@ -5920,13 +5923,13 @@
     </row>
     <row r="42" ht="15.75" customHeight="1">
       <c r="A42" s="11" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C42" s="7" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
@@ -5945,13 +5948,13 @@
     </row>
     <row r="43" ht="15.75" customHeight="1">
       <c r="A43" s="11" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D43" s="7"/>
       <c r="E43" s="7"/>
@@ -5970,13 +5973,13 @@
     </row>
     <row r="44" ht="15.75" customHeight="1">
       <c r="A44" s="11" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C44" s="7" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="D44" s="7"/>
       <c r="E44" s="7"/>
@@ -5995,13 +5998,13 @@
     </row>
     <row r="45" ht="15.75" customHeight="1">
       <c r="A45" s="11" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C45" s="7" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D45" s="7"/>
       <c r="E45" s="7"/>
@@ -6020,13 +6023,13 @@
     </row>
     <row r="46" ht="15.75" customHeight="1">
       <c r="A46" s="11" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B46" s="8" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C46" s="7" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D46" s="7"/>
       <c r="E46" s="7"/>
@@ -6045,13 +6048,13 @@
     </row>
     <row r="47" ht="15.75" customHeight="1">
       <c r="A47" s="11" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C47" s="7" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D47" s="7"/>
       <c r="E47" s="7"/>
@@ -6070,13 +6073,13 @@
     </row>
     <row r="48" ht="15.75" customHeight="1">
       <c r="A48" s="11" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B48" s="8" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C48" s="7" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="D48" s="7"/>
       <c r="E48" s="7"/>
@@ -6095,13 +6098,13 @@
     </row>
     <row r="49" ht="15.75" customHeight="1">
       <c r="A49" s="11" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B49" s="8" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C49" s="7" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D49" s="7"/>
       <c r="E49" s="7"/>
@@ -6120,20 +6123,18 @@
     </row>
     <row r="50" ht="15.75" customHeight="1">
       <c r="A50" s="11" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B50" s="8" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C50" s="7" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="D50" s="7"/>
       <c r="E50" s="7"/>
       <c r="F50" s="7"/>
-      <c r="G50" s="7" t="s">
-        <v>175</v>
-      </c>
+      <c r="G50" s="7"/>
       <c r="H50" s="7"/>
       <c r="I50" s="7"/>
       <c r="J50" s="7"/>
@@ -6192,8 +6193,8 @@
       <c r="I52" s="7"/>
       <c r="J52" s="7"/>
       <c r="K52" s="7"/>
-      <c r="L52" s="24"/>
-      <c r="M52" s="25" t="s">
+      <c r="L52" s="25"/>
+      <c r="M52" s="26" t="s">
         <v>183</v>
       </c>
       <c r="N52" s="11" t="s">
@@ -6255,7 +6256,7 @@
         <v>191</v>
       </c>
       <c r="N54" s="11" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="O54" s="7"/>
       <c r="P54" s="7"/>
@@ -6717,7 +6718,7 @@
       <c r="F72" s="7"/>
       <c r="G72" s="7"/>
       <c r="H72" s="7"/>
-      <c r="I72" s="26" t="s">
+      <c r="I72" s="27" t="s">
         <v>250</v>
       </c>
       <c r="J72" s="7"/>
@@ -6748,7 +6749,7 @@
       <c r="F73" s="7"/>
       <c r="G73" s="7"/>
       <c r="H73" s="7"/>
-      <c r="I73" s="26" t="s">
+      <c r="I73" s="27" t="s">
         <v>250</v>
       </c>
       <c r="J73" s="7"/>
@@ -6779,7 +6780,7 @@
       <c r="F74" s="7"/>
       <c r="G74" s="7"/>
       <c r="H74" s="7"/>
-      <c r="I74" s="26" t="s">
+      <c r="I74" s="27" t="s">
         <v>260</v>
       </c>
       <c r="J74" s="7"/>
@@ -6792,33 +6793,33 @@
       <c r="Q74" s="7"/>
     </row>
     <row r="75" ht="15.75" customHeight="1">
-      <c r="A75" s="27" t="s">
+      <c r="A75" s="28" t="s">
         <v>261</v>
       </c>
-      <c r="B75" s="28" t="s">
+      <c r="B75" s="29" t="s">
         <v>262</v>
       </c>
-      <c r="C75" s="28" t="s">
+      <c r="C75" s="29" t="s">
         <v>263</v>
       </c>
-      <c r="D75" s="28"/>
-      <c r="E75" s="28"/>
-      <c r="F75" s="28"/>
-      <c r="G75" s="28"/>
-      <c r="H75" s="28"/>
-      <c r="I75" s="28"/>
-      <c r="J75" s="28"/>
-      <c r="K75" s="28"/>
-      <c r="L75" s="28"/>
-      <c r="M75" s="28" t="s">
+      <c r="D75" s="29"/>
+      <c r="E75" s="29"/>
+      <c r="F75" s="29"/>
+      <c r="G75" s="29"/>
+      <c r="H75" s="29"/>
+      <c r="I75" s="29"/>
+      <c r="J75" s="29"/>
+      <c r="K75" s="29"/>
+      <c r="L75" s="29"/>
+      <c r="M75" s="29" t="s">
         <v>264</v>
       </c>
-      <c r="N75" s="27" t="s">
+      <c r="N75" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="O75" s="28"/>
-      <c r="P75" s="28"/>
-      <c r="Q75" s="28"/>
+      <c r="O75" s="29"/>
+      <c r="P75" s="29"/>
+      <c r="Q75" s="29"/>
     </row>
     <row r="76" ht="15.75" customHeight="1">
       <c r="A76" s="11" t="s">
@@ -6837,7 +6838,7 @@
       <c r="F76" s="7"/>
       <c r="G76" s="7"/>
       <c r="H76" s="7"/>
-      <c r="I76" s="26" t="s">
+      <c r="I76" s="27" t="s">
         <v>268</v>
       </c>
       <c r="J76" s="7"/>
@@ -6853,7 +6854,7 @@
       <c r="A77" s="11" t="s">
         <v>269</v>
       </c>
-      <c r="B77" s="29" t="s">
+      <c r="B77" s="30" t="s">
         <v>270</v>
       </c>
       <c r="C77" s="7" t="s">
@@ -6868,11 +6869,11 @@
       <c r="J77" s="7"/>
       <c r="K77" s="7"/>
       <c r="L77" s="7"/>
-      <c r="M77" s="30" t="s">
+      <c r="M77" s="31" t="s">
         <v>272</v>
       </c>
       <c r="N77" s="11" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="O77" s="7"/>
       <c r="P77" s="7"/>
@@ -6942,7 +6943,7 @@
       <c r="G80" s="7"/>
       <c r="H80" s="7"/>
       <c r="I80" s="7"/>
-      <c r="J80" s="23">
+      <c r="J80" s="24">
         <v>229.0</v>
       </c>
       <c r="K80" s="7"/>
@@ -6969,7 +6970,7 @@
       <c r="G81" s="7"/>
       <c r="H81" s="7"/>
       <c r="I81" s="7"/>
-      <c r="J81" s="23">
+      <c r="J81" s="24">
         <v>229.0</v>
       </c>
       <c r="K81" s="7"/>
@@ -6998,7 +6999,7 @@
       <c r="G82" s="7"/>
       <c r="H82" s="7"/>
       <c r="I82" s="7"/>
-      <c r="J82" s="23">
+      <c r="J82" s="24">
         <v>229.0</v>
       </c>
       <c r="K82" s="7"/>
@@ -7054,8 +7055,8 @@
       <c r="I84" s="7"/>
       <c r="J84" s="7"/>
       <c r="K84" s="7"/>
-      <c r="L84" s="31"/>
-      <c r="M84" s="31"/>
+      <c r="L84" s="32"/>
+      <c r="M84" s="32"/>
       <c r="N84" s="11"/>
       <c r="O84" s="7"/>
       <c r="P84" s="7"/>
@@ -7112,138 +7113,138 @@
       <c r="Q86" s="7"/>
     </row>
     <row r="87" ht="15.75" customHeight="1">
-      <c r="A87" s="32" t="s">
+      <c r="A87" s="33" t="s">
         <v>292</v>
       </c>
-      <c r="B87" s="33" t="s">
+      <c r="B87" s="34" t="s">
         <v>293</v>
       </c>
-      <c r="C87" s="34" t="s">
+      <c r="C87" s="35" t="s">
         <v>86</v>
       </c>
-      <c r="D87" s="33"/>
-      <c r="E87" s="35"/>
-      <c r="F87" s="33"/>
-      <c r="G87" s="33"/>
-      <c r="H87" s="33"/>
-      <c r="I87" s="33"/>
-      <c r="J87" s="36">
+      <c r="D87" s="34"/>
+      <c r="E87" s="36"/>
+      <c r="F87" s="34"/>
+      <c r="G87" s="34"/>
+      <c r="H87" s="34"/>
+      <c r="I87" s="34"/>
+      <c r="J87" s="37">
         <v>229.0</v>
       </c>
-      <c r="K87" s="33"/>
-      <c r="L87" s="33" t="s">
-        <v>121</v>
-      </c>
-      <c r="M87" s="33"/>
-      <c r="N87" s="32"/>
-      <c r="O87" s="33"/>
-      <c r="P87" s="33"/>
-      <c r="Q87" s="33"/>
+      <c r="K87" s="34"/>
+      <c r="L87" s="34" t="s">
+        <v>122</v>
+      </c>
+      <c r="M87" s="34"/>
+      <c r="N87" s="33"/>
+      <c r="O87" s="34"/>
+      <c r="P87" s="34"/>
+      <c r="Q87" s="34"/>
     </row>
     <row r="88" ht="15.75" customHeight="1">
-      <c r="A88" s="32" t="s">
+      <c r="A88" s="33" t="s">
         <v>294</v>
       </c>
-      <c r="B88" s="33" t="s">
+      <c r="B88" s="34" t="s">
         <v>295</v>
       </c>
-      <c r="C88" s="34" t="s">
+      <c r="C88" s="35" t="s">
         <v>86</v>
       </c>
-      <c r="D88" s="33"/>
-      <c r="E88" s="33"/>
-      <c r="F88" s="33"/>
-      <c r="G88" s="33"/>
-      <c r="H88" s="33"/>
-      <c r="I88" s="33"/>
-      <c r="J88" s="36">
+      <c r="D88" s="34"/>
+      <c r="E88" s="34"/>
+      <c r="F88" s="34"/>
+      <c r="G88" s="34"/>
+      <c r="H88" s="34"/>
+      <c r="I88" s="34"/>
+      <c r="J88" s="37">
         <v>229.0</v>
       </c>
-      <c r="K88" s="33"/>
-      <c r="L88" s="33" t="s">
-        <v>126</v>
-      </c>
-      <c r="M88" s="33"/>
-      <c r="N88" s="32"/>
-      <c r="O88" s="33"/>
-      <c r="P88" s="33"/>
-      <c r="Q88" s="33"/>
+      <c r="K88" s="34"/>
+      <c r="L88" s="34" t="s">
+        <v>127</v>
+      </c>
+      <c r="M88" s="34"/>
+      <c r="N88" s="33"/>
+      <c r="O88" s="34"/>
+      <c r="P88" s="34"/>
+      <c r="Q88" s="34"/>
     </row>
     <row r="89" ht="15.75" customHeight="1">
-      <c r="A89" s="32" t="s">
+      <c r="A89" s="33" t="s">
         <v>296</v>
       </c>
-      <c r="B89" s="33" t="s">
+      <c r="B89" s="34" t="s">
         <v>297</v>
       </c>
-      <c r="C89" s="34" t="s">
+      <c r="C89" s="35" t="s">
         <v>86</v>
       </c>
-      <c r="D89" s="33"/>
-      <c r="E89" s="35"/>
-      <c r="F89" s="33"/>
-      <c r="G89" s="33"/>
-      <c r="H89" s="33"/>
-      <c r="I89" s="33"/>
-      <c r="J89" s="36">
+      <c r="D89" s="34"/>
+      <c r="E89" s="36"/>
+      <c r="F89" s="34"/>
+      <c r="G89" s="34"/>
+      <c r="H89" s="34"/>
+      <c r="I89" s="34"/>
+      <c r="J89" s="37">
         <v>229.0</v>
       </c>
-      <c r="K89" s="33"/>
-      <c r="L89" s="32" t="s">
-        <v>121</v>
-      </c>
-      <c r="M89" s="32"/>
-      <c r="N89" s="32"/>
-      <c r="O89" s="33"/>
-      <c r="P89" s="33"/>
-      <c r="Q89" s="33"/>
+      <c r="K89" s="34"/>
+      <c r="L89" s="33" t="s">
+        <v>122</v>
+      </c>
+      <c r="M89" s="33"/>
+      <c r="N89" s="33"/>
+      <c r="O89" s="34"/>
+      <c r="P89" s="34"/>
+      <c r="Q89" s="34"/>
     </row>
     <row r="90" ht="15.75" customHeight="1">
-      <c r="A90" s="32" t="s">
+      <c r="A90" s="33" t="s">
         <v>298</v>
       </c>
-      <c r="B90" s="33" t="s">
+      <c r="B90" s="34" t="s">
         <v>299</v>
       </c>
-      <c r="C90" s="34" t="s">
+      <c r="C90" s="35" t="s">
         <v>86</v>
       </c>
-      <c r="D90" s="33"/>
-      <c r="E90" s="35"/>
-      <c r="F90" s="33"/>
-      <c r="G90" s="33"/>
-      <c r="H90" s="33"/>
-      <c r="I90" s="33"/>
-      <c r="J90" s="36">
+      <c r="D90" s="34"/>
+      <c r="E90" s="36"/>
+      <c r="F90" s="34"/>
+      <c r="G90" s="34"/>
+      <c r="H90" s="34"/>
+      <c r="I90" s="34"/>
+      <c r="J90" s="37">
         <v>229.0</v>
       </c>
-      <c r="K90" s="33"/>
-      <c r="L90" s="32" t="s">
-        <v>126</v>
-      </c>
-      <c r="M90" s="32"/>
-      <c r="N90" s="32"/>
-      <c r="O90" s="33"/>
-      <c r="P90" s="33"/>
-      <c r="Q90" s="33"/>
+      <c r="K90" s="34"/>
+      <c r="L90" s="33" t="s">
+        <v>127</v>
+      </c>
+      <c r="M90" s="33"/>
+      <c r="N90" s="33"/>
+      <c r="O90" s="34"/>
+      <c r="P90" s="34"/>
+      <c r="Q90" s="34"/>
     </row>
     <row r="91" ht="15.75" customHeight="1">
-      <c r="A91" s="37" t="s">
+      <c r="A91" s="38" t="s">
         <v>300</v>
       </c>
-      <c r="B91" s="38" t="s">
+      <c r="B91" s="39" t="s">
         <v>301</v>
       </c>
-      <c r="C91" s="38" t="s">
+      <c r="C91" s="39" t="s">
         <v>302</v>
       </c>
-      <c r="D91" s="38"/>
-      <c r="E91" s="38"/>
-      <c r="F91" s="38"/>
-      <c r="G91" s="38"/>
-      <c r="H91" s="38"/>
-      <c r="I91" s="38"/>
-      <c r="J91" s="38"/>
+      <c r="D91" s="39"/>
+      <c r="E91" s="39"/>
+      <c r="F91" s="39"/>
+      <c r="G91" s="39"/>
+      <c r="H91" s="39"/>
+      <c r="I91" s="39"/>
+      <c r="J91" s="39"/>
       <c r="K91" s="11"/>
       <c r="L91" s="11"/>
       <c r="M91" s="11" t="s">
@@ -7257,62 +7258,62 @@
       <c r="Q91" s="7"/>
     </row>
     <row r="92" ht="15.75" customHeight="1">
-      <c r="A92" s="32" t="s">
-        <v>107</v>
-      </c>
-      <c r="B92" s="33" t="s">
+      <c r="A92" s="33" t="s">
+        <v>108</v>
+      </c>
+      <c r="B92" s="34" t="s">
         <v>304</v>
       </c>
-      <c r="C92" s="34" t="s">
+      <c r="C92" s="35" t="s">
         <v>86</v>
       </c>
-      <c r="D92" s="33"/>
-      <c r="E92" s="33"/>
-      <c r="F92" s="33"/>
-      <c r="G92" s="33"/>
-      <c r="H92" s="33"/>
-      <c r="I92" s="33"/>
-      <c r="J92" s="36">
+      <c r="D92" s="34"/>
+      <c r="E92" s="34"/>
+      <c r="F92" s="34"/>
+      <c r="G92" s="34"/>
+      <c r="H92" s="34"/>
+      <c r="I92" s="34"/>
+      <c r="J92" s="37">
         <v>229.0</v>
       </c>
-      <c r="K92" s="33"/>
-      <c r="L92" s="33" t="s">
-        <v>104</v>
-      </c>
-      <c r="M92" s="33"/>
-      <c r="N92" s="32"/>
-      <c r="O92" s="33"/>
-      <c r="P92" s="33"/>
-      <c r="Q92" s="33"/>
+      <c r="K92" s="34"/>
+      <c r="L92" s="34" t="s">
+        <v>105</v>
+      </c>
+      <c r="M92" s="34"/>
+      <c r="N92" s="33"/>
+      <c r="O92" s="34"/>
+      <c r="P92" s="34"/>
+      <c r="Q92" s="34"/>
     </row>
     <row r="93" ht="15.75" customHeight="1">
-      <c r="A93" s="32" t="s">
-        <v>111</v>
-      </c>
-      <c r="B93" s="33" t="s">
+      <c r="A93" s="33" t="s">
+        <v>112</v>
+      </c>
+      <c r="B93" s="34" t="s">
         <v>305</v>
       </c>
-      <c r="C93" s="33" t="s">
+      <c r="C93" s="34" t="s">
         <v>306</v>
       </c>
-      <c r="D93" s="33"/>
-      <c r="E93" s="33"/>
-      <c r="F93" s="33"/>
-      <c r="G93" s="33"/>
-      <c r="H93" s="33"/>
-      <c r="I93" s="33"/>
-      <c r="J93" s="36">
+      <c r="D93" s="34"/>
+      <c r="E93" s="34"/>
+      <c r="F93" s="34"/>
+      <c r="G93" s="34"/>
+      <c r="H93" s="34"/>
+      <c r="I93" s="34"/>
+      <c r="J93" s="37">
         <v>229.0</v>
       </c>
-      <c r="K93" s="33"/>
-      <c r="L93" s="33" t="s">
-        <v>108</v>
-      </c>
-      <c r="M93" s="33"/>
-      <c r="N93" s="32"/>
-      <c r="O93" s="33"/>
-      <c r="P93" s="33"/>
-      <c r="Q93" s="33"/>
+      <c r="K93" s="34"/>
+      <c r="L93" s="34" t="s">
+        <v>109</v>
+      </c>
+      <c r="M93" s="34"/>
+      <c r="N93" s="33"/>
+      <c r="O93" s="34"/>
+      <c r="P93" s="34"/>
+      <c r="Q93" s="34"/>
     </row>
     <row r="94" ht="15.75" customHeight="1"/>
     <row r="95" ht="15.75" customHeight="1"/>
@@ -8191,16 +8192,16 @@
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="39" t="s">
+      <c r="B1" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="39" t="s">
+      <c r="C1" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="39" t="s">
+      <c r="D1" s="40" t="s">
         <v>12</v>
       </c>
     </row>
@@ -8276,7 +8277,7 @@
       <c r="C7" s="8" t="s">
         <v>325</v>
       </c>
-      <c r="D7" s="40" t="s">
+      <c r="D7" s="41" t="s">
         <v>326</v>
       </c>
     </row>
@@ -8290,7 +8291,7 @@
       <c r="C8" s="8" t="s">
         <v>309</v>
       </c>
-      <c r="D8" s="40" t="s">
+      <c r="D8" s="41" t="s">
         <v>326</v>
       </c>
     </row>
@@ -8304,7 +8305,7 @@
       <c r="C9" s="8" t="s">
         <v>330</v>
       </c>
-      <c r="D9" s="41" t="s">
+      <c r="D9" s="42" t="s">
         <v>331</v>
       </c>
     </row>
@@ -8318,7 +8319,7 @@
       <c r="C10" s="8" t="s">
         <v>334</v>
       </c>
-      <c r="D10" s="40" t="s">
+      <c r="D10" s="41" t="s">
         <v>326</v>
       </c>
     </row>
@@ -8332,19 +8333,19 @@
       <c r="C11" s="8" t="s">
         <v>337</v>
       </c>
-      <c r="D11" s="40"/>
+      <c r="D11" s="41"/>
     </row>
     <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="14" t="s">
         <v>338</v>
       </c>
-      <c r="B12" s="40" t="s">
+      <c r="B12" s="41" t="s">
         <v>339</v>
       </c>
-      <c r="C12" s="40" t="s">
+      <c r="C12" s="41" t="s">
         <v>340</v>
       </c>
-      <c r="D12" s="40"/>
+      <c r="D12" s="41"/>
     </row>
     <row r="13" ht="15.75" customHeight="1">
       <c r="A13" s="14" t="s">
@@ -8353,10 +8354,10 @@
       <c r="B13" s="8" t="s">
         <v>342</v>
       </c>
-      <c r="C13" s="40" t="s">
+      <c r="C13" s="41" t="s">
         <v>343</v>
       </c>
-      <c r="D13" s="40"/>
+      <c r="D13" s="41"/>
     </row>
     <row r="14" ht="15.75" customHeight="1">
       <c r="A14" s="14" t="s">
@@ -8365,10 +8366,10 @@
       <c r="B14" s="8" t="s">
         <v>345</v>
       </c>
-      <c r="C14" s="40" t="s">
+      <c r="C14" s="41" t="s">
         <v>346</v>
       </c>
-      <c r="D14" s="40"/>
+      <c r="D14" s="41"/>
     </row>
     <row r="15" ht="15.75" customHeight="1">
       <c r="A15" s="14" t="s">
@@ -8377,10 +8378,10 @@
       <c r="B15" s="8" t="s">
         <v>348</v>
       </c>
-      <c r="C15" s="40" t="s">
+      <c r="C15" s="41" t="s">
         <v>349</v>
       </c>
-      <c r="D15" s="40"/>
+      <c r="D15" s="41"/>
     </row>
     <row r="16" ht="15.75" customHeight="1">
       <c r="A16" s="14" t="s">
@@ -8389,10 +8390,10 @@
       <c r="B16" s="8" t="s">
         <v>351</v>
       </c>
-      <c r="C16" s="40" t="s">
+      <c r="C16" s="41" t="s">
         <v>352</v>
       </c>
-      <c r="D16" s="40"/>
+      <c r="D16" s="41"/>
     </row>
     <row r="17" ht="15.75" customHeight="1">
       <c r="A17" s="14" t="s">
@@ -8401,10 +8402,10 @@
       <c r="B17" s="8" t="s">
         <v>354</v>
       </c>
-      <c r="C17" s="40" t="s">
+      <c r="C17" s="41" t="s">
         <v>355</v>
       </c>
-      <c r="D17" s="40"/>
+      <c r="D17" s="41"/>
     </row>
     <row r="18" ht="15.75" customHeight="1">
       <c r="A18" s="14" t="s">
@@ -8413,10 +8414,10 @@
       <c r="B18" s="8" t="s">
         <v>357</v>
       </c>
-      <c r="C18" s="40" t="s">
+      <c r="C18" s="41" t="s">
         <v>358</v>
       </c>
-      <c r="D18" s="40"/>
+      <c r="D18" s="41"/>
     </row>
     <row r="19" ht="15.75" customHeight="1">
       <c r="A19" s="14" t="s">
@@ -8425,10 +8426,10 @@
       <c r="B19" s="8" t="s">
         <v>360</v>
       </c>
-      <c r="C19" s="40" t="s">
+      <c r="C19" s="41" t="s">
         <v>361</v>
       </c>
-      <c r="D19" s="40"/>
+      <c r="D19" s="41"/>
     </row>
     <row r="20" ht="15.75" customHeight="1">
       <c r="A20" s="14" t="s">
@@ -8437,10 +8438,10 @@
       <c r="B20" s="8" t="s">
         <v>363</v>
       </c>
-      <c r="C20" s="42" t="s">
+      <c r="C20" s="43" t="s">
         <v>330</v>
       </c>
-      <c r="D20" s="40"/>
+      <c r="D20" s="41"/>
     </row>
     <row r="21" ht="15.75" customHeight="1">
       <c r="A21" s="14" t="s">
@@ -8449,10 +8450,10 @@
       <c r="B21" s="8" t="s">
         <v>365</v>
       </c>
-      <c r="C21" s="42" t="s">
+      <c r="C21" s="43" t="s">
         <v>366</v>
       </c>
-      <c r="D21" s="40"/>
+      <c r="D21" s="41"/>
     </row>
     <row r="22" ht="15.75" customHeight="1">
       <c r="A22" s="14" t="s">
@@ -8461,10 +8462,10 @@
       <c r="B22" s="8" t="s">
         <v>368</v>
       </c>
-      <c r="C22" s="43" t="s">
+      <c r="C22" s="44" t="s">
         <v>369</v>
       </c>
-      <c r="D22" s="40" t="s">
+      <c r="D22" s="41" t="s">
         <v>320</v>
       </c>
     </row>
@@ -8475,10 +8476,10 @@
       <c r="B23" s="7" t="s">
         <v>371</v>
       </c>
-      <c r="C23" s="44" t="s">
+      <c r="C23" s="45" t="s">
         <v>372</v>
       </c>
-      <c r="D23" s="40"/>
+      <c r="D23" s="41"/>
     </row>
     <row r="24" ht="15.75" customHeight="1">
       <c r="A24" s="14" t="s">
@@ -8487,10 +8488,10 @@
       <c r="B24" s="7" t="s">
         <v>374</v>
       </c>
-      <c r="C24" s="44" t="s">
+      <c r="C24" s="45" t="s">
         <v>375</v>
       </c>
-      <c r="D24" s="40"/>
+      <c r="D24" s="41"/>
     </row>
     <row r="25" ht="15.75" customHeight="1">
       <c r="A25" s="14" t="s">
@@ -8499,10 +8500,10 @@
       <c r="B25" s="7" t="s">
         <v>377</v>
       </c>
-      <c r="C25" s="44" t="s">
+      <c r="C25" s="45" t="s">
         <v>378</v>
       </c>
-      <c r="D25" s="40" t="s">
+      <c r="D25" s="41" t="s">
         <v>320</v>
       </c>
     </row>
@@ -8510,13 +8511,13 @@
       <c r="A26" s="14" t="s">
         <v>379</v>
       </c>
-      <c r="B26" s="40" t="s">
+      <c r="B26" s="41" t="s">
         <v>380</v>
       </c>
-      <c r="C26" s="40" t="s">
+      <c r="C26" s="41" t="s">
         <v>381</v>
       </c>
-      <c r="D26" s="40" t="s">
+      <c r="D26" s="41" t="s">
         <v>338</v>
       </c>
     </row>
@@ -8524,229 +8525,229 @@
       <c r="A27" s="14" t="s">
         <v>382</v>
       </c>
-      <c r="B27" s="40" t="s">
+      <c r="B27" s="41" t="s">
         <v>383</v>
       </c>
-      <c r="C27" s="40" t="s">
+      <c r="C27" s="41" t="s">
         <v>384</v>
       </c>
-      <c r="D27" s="40"/>
+      <c r="D27" s="41"/>
     </row>
     <row r="28" ht="15.75" customHeight="1">
       <c r="A28" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="B28" s="40" t="s">
+      <c r="B28" s="41" t="s">
         <v>385</v>
       </c>
-      <c r="C28" s="40" t="s">
+      <c r="C28" s="41" t="s">
         <v>386</v>
       </c>
-      <c r="D28" s="40"/>
+      <c r="D28" s="41"/>
     </row>
     <row r="29" ht="15.75" customHeight="1">
-      <c r="A29" s="29" t="s">
+      <c r="A29" s="30" t="s">
         <v>387</v>
       </c>
       <c r="B29" s="15" t="s">
         <v>388</v>
       </c>
-      <c r="C29" s="29" t="s">
+      <c r="C29" s="30" t="s">
         <v>389</v>
       </c>
-      <c r="D29" s="29"/>
+      <c r="D29" s="30"/>
     </row>
     <row r="30" ht="15.75" customHeight="1">
-      <c r="A30" s="29" t="s">
+      <c r="A30" s="30" t="s">
         <v>390</v>
       </c>
       <c r="B30" s="15" t="s">
         <v>391</v>
       </c>
-      <c r="C30" s="29" t="s">
+      <c r="C30" s="30" t="s">
         <v>392</v>
       </c>
-      <c r="D30" s="29"/>
+      <c r="D30" s="30"/>
     </row>
     <row r="31" ht="15.75" customHeight="1">
-      <c r="A31" s="29" t="s">
+      <c r="A31" s="30" t="s">
         <v>393</v>
       </c>
       <c r="B31" s="15" t="s">
         <v>394</v>
       </c>
-      <c r="C31" s="29" t="s">
+      <c r="C31" s="30" t="s">
         <v>395</v>
       </c>
-      <c r="D31" s="29"/>
+      <c r="D31" s="30"/>
     </row>
     <row r="32" ht="15.75" customHeight="1">
-      <c r="A32" s="29" t="s">
+      <c r="A32" s="30" t="s">
         <v>396</v>
       </c>
       <c r="B32" s="15" t="s">
         <v>397</v>
       </c>
-      <c r="C32" s="29" t="s">
+      <c r="C32" s="30" t="s">
         <v>398</v>
       </c>
-      <c r="D32" s="29"/>
+      <c r="D32" s="30"/>
     </row>
     <row r="33" ht="15.75" customHeight="1">
-      <c r="A33" s="29" t="s">
+      <c r="A33" s="30" t="s">
         <v>399</v>
       </c>
       <c r="B33" s="15" t="s">
         <v>400</v>
       </c>
-      <c r="C33" s="29" t="s">
+      <c r="C33" s="30" t="s">
         <v>401</v>
       </c>
-      <c r="D33" s="29"/>
+      <c r="D33" s="30"/>
     </row>
     <row r="34" ht="15.75" customHeight="1">
-      <c r="A34" s="29" t="s">
+      <c r="A34" s="30" t="s">
         <v>402</v>
       </c>
       <c r="B34" s="15" t="s">
         <v>403</v>
       </c>
-      <c r="C34" s="29" t="s">
+      <c r="C34" s="30" t="s">
         <v>404</v>
       </c>
-      <c r="D34" s="29"/>
+      <c r="D34" s="30"/>
     </row>
     <row r="35" ht="15.75" customHeight="1">
-      <c r="A35" s="29" t="s">
+      <c r="A35" s="30" t="s">
         <v>405</v>
       </c>
       <c r="B35" s="15" t="s">
         <v>406</v>
       </c>
-      <c r="C35" s="29" t="s">
+      <c r="C35" s="30" t="s">
         <v>407</v>
       </c>
-      <c r="D35" s="29"/>
+      <c r="D35" s="30"/>
     </row>
     <row r="36" ht="15.75" customHeight="1">
-      <c r="A36" s="29" t="s">
+      <c r="A36" s="30" t="s">
         <v>408</v>
       </c>
       <c r="B36" s="15" t="s">
         <v>409</v>
       </c>
-      <c r="C36" s="29" t="s">
+      <c r="C36" s="30" t="s">
         <v>410</v>
       </c>
-      <c r="D36" s="29"/>
+      <c r="D36" s="30"/>
     </row>
     <row r="37" ht="15.75" customHeight="1">
-      <c r="A37" s="29" t="s">
+      <c r="A37" s="30" t="s">
         <v>411</v>
       </c>
       <c r="B37" s="15" t="s">
         <v>412</v>
       </c>
-      <c r="C37" s="29" t="s">
+      <c r="C37" s="30" t="s">
         <v>413</v>
       </c>
-      <c r="D37" s="29"/>
+      <c r="D37" s="30"/>
     </row>
     <row r="38" ht="15.75" customHeight="1">
-      <c r="A38" s="29" t="s">
+      <c r="A38" s="30" t="s">
         <v>414</v>
       </c>
       <c r="B38" s="15" t="s">
         <v>415</v>
       </c>
-      <c r="C38" s="29" t="s">
+      <c r="C38" s="30" t="s">
         <v>416</v>
       </c>
-      <c r="D38" s="29"/>
+      <c r="D38" s="30"/>
     </row>
     <row r="39" ht="15.75" customHeight="1">
-      <c r="A39" s="23">
+      <c r="A39" s="24">
         <v>54.0</v>
       </c>
       <c r="B39" s="7" t="s">
         <v>417</v>
       </c>
-      <c r="C39" s="45" t="s">
+      <c r="C39" s="46" t="s">
         <v>418</v>
       </c>
-      <c r="D39" s="23"/>
+      <c r="D39" s="24"/>
     </row>
     <row r="40" ht="15.75" customHeight="1">
-      <c r="A40" s="23">
+      <c r="A40" s="24">
         <v>55.0</v>
       </c>
       <c r="B40" s="7" t="s">
         <v>419</v>
       </c>
-      <c r="C40" s="45" t="s">
+      <c r="C40" s="46" t="s">
         <v>420</v>
       </c>
       <c r="D40" s="7"/>
     </row>
     <row r="41" ht="15.75" customHeight="1">
-      <c r="A41" s="23">
+      <c r="A41" s="24">
         <v>56.0</v>
       </c>
       <c r="B41" s="7" t="s">
         <v>421</v>
       </c>
-      <c r="C41" s="45" t="s">
+      <c r="C41" s="46" t="s">
         <v>422</v>
       </c>
-      <c r="D41" s="23"/>
+      <c r="D41" s="24"/>
     </row>
     <row r="42" ht="15.75" customHeight="1">
-      <c r="A42" s="23">
+      <c r="A42" s="24">
         <v>116.0</v>
       </c>
       <c r="B42" s="7" t="s">
         <v>321</v>
       </c>
-      <c r="C42" s="46" t="s">
+      <c r="C42" s="47" t="s">
         <v>423</v>
       </c>
-      <c r="D42" s="40"/>
+      <c r="D42" s="41"/>
     </row>
     <row r="43" ht="15.75" customHeight="1">
-      <c r="A43" s="23" t="s">
+      <c r="A43" s="24" t="s">
         <v>424</v>
       </c>
       <c r="B43" s="7" t="s">
         <v>425</v>
       </c>
-      <c r="C43" s="46" t="s">
+      <c r="C43" s="47" t="s">
         <v>426</v>
       </c>
-      <c r="D43" s="40"/>
+      <c r="D43" s="41"/>
     </row>
     <row r="44" ht="15.75" customHeight="1">
-      <c r="A44" s="23" t="s">
+      <c r="A44" s="24" t="s">
         <v>427</v>
       </c>
       <c r="B44" s="7" t="s">
         <v>428</v>
       </c>
-      <c r="C44" s="46" t="s">
+      <c r="C44" s="47" t="s">
         <v>429</v>
       </c>
-      <c r="D44" s="40"/>
+      <c r="D44" s="41"/>
     </row>
     <row r="45" ht="15.75" customHeight="1">
-      <c r="A45" s="23" t="s">
+      <c r="A45" s="24" t="s">
         <v>430</v>
       </c>
       <c r="B45" s="7" t="s">
         <v>431</v>
       </c>
-      <c r="C45" s="47" t="s">
+      <c r="C45" s="48" t="s">
         <v>432</v>
       </c>
-      <c r="D45" s="40"/>
+      <c r="D45" s="41"/>
     </row>
     <row r="46" ht="15.75" customHeight="1"/>
     <row r="47" ht="15.75" customHeight="1"/>
@@ -9762,7 +9763,7 @@
       <c r="E2" s="11" t="s">
         <v>277</v>
       </c>
-      <c r="F2" s="23">
+      <c r="F2" s="24">
         <v>4.0</v>
       </c>
       <c r="G2" s="7"/>
@@ -10781,7 +10782,7 @@
       <c r="D1" s="4" t="s">
         <v>440</v>
       </c>
-      <c r="E1" s="48" t="s">
+      <c r="E1" s="49" t="s">
         <v>441</v>
       </c>
       <c r="F1" s="4" t="s">
@@ -10796,10 +10797,10 @@
       <c r="I1" s="4" t="s">
         <v>444</v>
       </c>
-      <c r="J1" s="49" t="s">
+      <c r="J1" s="50" t="s">
         <v>445</v>
       </c>
-      <c r="K1" s="50" t="s">
+      <c r="K1" s="51" t="s">
         <v>446</v>
       </c>
       <c r="L1" s="51" t="s">
@@ -10808,7 +10809,7 @@
       <c r="M1" s="52" t="s">
         <v>448</v>
       </c>
-      <c r="N1" s="31" t="s">
+      <c r="N1" s="32" t="s">
         <v>436</v>
       </c>
     </row>
@@ -10824,7 +10825,7 @@
       </c>
       <c r="D2" s="21"/>
       <c r="E2" s="55" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="F2" s="21" t="s">
         <v>438</v>
@@ -10843,31 +10844,31 @@
       <c r="N2" s="58"/>
     </row>
     <row r="3" ht="15.75" customHeight="1">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="33" t="s">
         <v>452</v>
       </c>
-      <c r="B3" s="33" t="s">
+      <c r="B3" s="34" t="s">
         <v>453</v>
       </c>
       <c r="C3" s="20" t="s">
         <v>454</v>
       </c>
-      <c r="D3" s="33"/>
+      <c r="D3" s="34"/>
       <c r="E3" s="59" t="s">
         <v>81</v>
       </c>
-      <c r="F3" s="33" t="s">
+      <c r="F3" s="34" t="s">
         <v>439</v>
       </c>
-      <c r="G3" s="32" t="s">
+      <c r="G3" s="33" t="s">
         <v>455</v>
       </c>
-      <c r="H3" s="33"/>
-      <c r="I3" s="33"/>
-      <c r="J3" s="33"/>
-      <c r="K3" s="36"/>
-      <c r="L3" s="36" t="s">
-        <v>125</v>
+      <c r="H3" s="34"/>
+      <c r="I3" s="34"/>
+      <c r="J3" s="34"/>
+      <c r="K3" s="37"/>
+      <c r="L3" s="37" t="s">
+        <v>126</v>
       </c>
       <c r="M3" s="60" t="s">
         <v>456</v>
@@ -10875,65 +10876,65 @@
       <c r="N3" s="61"/>
     </row>
     <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" s="32" t="s">
+      <c r="A4" s="33" t="s">
         <v>457</v>
       </c>
-      <c r="B4" s="33" t="s">
+      <c r="B4" s="34" t="s">
         <v>458</v>
       </c>
       <c r="C4" s="20" t="s">
         <v>454</v>
       </c>
-      <c r="D4" s="33"/>
+      <c r="D4" s="34"/>
       <c r="E4" s="59" t="s">
-        <v>89</v>
-      </c>
-      <c r="F4" s="33" t="s">
+        <v>90</v>
+      </c>
+      <c r="F4" s="34" t="s">
         <v>455</v>
       </c>
-      <c r="G4" s="32" t="s">
+      <c r="G4" s="33" t="s">
         <v>459</v>
       </c>
-      <c r="H4" s="33"/>
-      <c r="I4" s="33"/>
-      <c r="J4" s="33"/>
-      <c r="K4" s="62"/>
-      <c r="L4" s="36" t="s">
+      <c r="H4" s="34"/>
+      <c r="I4" s="34"/>
+      <c r="J4" s="34"/>
+      <c r="K4" s="37"/>
+      <c r="L4" s="37" t="s">
         <v>460</v>
       </c>
-      <c r="M4" s="63" t="s">
+      <c r="M4" s="60" t="s">
         <v>461</v>
       </c>
       <c r="N4" s="61"/>
     </row>
     <row r="5" ht="15.75" customHeight="1">
-      <c r="A5" s="32" t="s">
+      <c r="A5" s="33" t="s">
         <v>462</v>
       </c>
-      <c r="B5" s="33" t="s">
+      <c r="B5" s="34" t="s">
         <v>463</v>
       </c>
       <c r="C5" s="20" t="s">
         <v>454</v>
       </c>
-      <c r="D5" s="33"/>
+      <c r="D5" s="34"/>
       <c r="E5" s="59" t="s">
-        <v>89</v>
-      </c>
-      <c r="F5" s="33" t="s">
+        <v>90</v>
+      </c>
+      <c r="F5" s="34" t="s">
         <v>455</v>
       </c>
-      <c r="G5" s="32" t="s">
+      <c r="G5" s="33" t="s">
         <v>464</v>
       </c>
-      <c r="H5" s="33"/>
-      <c r="I5" s="33"/>
-      <c r="J5" s="33"/>
-      <c r="K5" s="62"/>
-      <c r="L5" s="36" t="s">
+      <c r="H5" s="34"/>
+      <c r="I5" s="34"/>
+      <c r="J5" s="34"/>
+      <c r="K5" s="37"/>
+      <c r="L5" s="37" t="s">
         <v>460</v>
       </c>
-      <c r="M5" s="63" t="s">
+      <c r="M5" s="60" t="s">
         <v>465</v>
       </c>
       <c r="N5" s="61"/>
@@ -13152,53 +13153,53 @@
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
-      <c r="A1" s="64" t="s">
+      <c r="A1" s="62" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="64" t="s">
+      <c r="B1" s="62" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="64" t="s">
+      <c r="C1" s="62" t="s">
         <v>440</v>
       </c>
-      <c r="D1" s="64" t="s">
+      <c r="D1" s="62" t="s">
         <v>497</v>
       </c>
-      <c r="E1" s="64" t="s">
+      <c r="E1" s="62" t="s">
         <v>498</v>
       </c>
-      <c r="F1" s="65" t="s">
+      <c r="F1" s="62" t="s">
         <v>499</v>
       </c>
-      <c r="G1" s="65" t="s">
-        <v>436</v>
-      </c>
-      <c r="H1" s="65" t="s">
+      <c r="G1" s="63" t="s">
+        <v>500</v>
+      </c>
+      <c r="H1" s="62" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" ht="120.75" customHeight="1">
-      <c r="A2" s="65" t="s">
-        <v>500</v>
-      </c>
-      <c r="B2" s="65" t="s">
+      <c r="A2" s="64" t="s">
         <v>501</v>
       </c>
-      <c r="C2" s="65"/>
-      <c r="D2" s="66" t="s">
+      <c r="B2" s="64" t="s">
+        <v>502</v>
+      </c>
+      <c r="C2" s="64"/>
+      <c r="D2" s="65" t="s">
         <v>437</v>
       </c>
-      <c r="E2" s="67" t="s">
-        <v>502</v>
-      </c>
-      <c r="F2" s="65" t="s">
+      <c r="E2" s="66" t="s">
         <v>503</v>
       </c>
-      <c r="G2" s="65" t="s">
+      <c r="F2" s="64" t="s">
         <v>504</v>
       </c>
-      <c r="H2" s="65" t="s">
+      <c r="G2" s="64" t="s">
         <v>505</v>
+      </c>
+      <c r="H2" s="64" t="s">
+        <v>506</v>
       </c>
     </row>
   </sheetData>
@@ -13222,129 +13223,129 @@
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
-      <c r="A1" s="68" t="s">
+      <c r="A1" s="67" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" s="69" t="s">
-        <v>508</v>
-      </c>
-      <c r="C2" s="70" t="s">
+      <c r="A2" s="68" t="s">
         <v>509</v>
       </c>
+      <c r="C2" s="69" t="s">
+        <v>510</v>
+      </c>
     </row>
     <row r="3" ht="15.75" customHeight="1">
-      <c r="A3" s="71" t="s">
-        <v>510</v>
-      </c>
-      <c r="C3" s="70" t="s">
+      <c r="A3" s="70" t="s">
         <v>511</v>
       </c>
+      <c r="C3" s="69" t="s">
+        <v>512</v>
+      </c>
     </row>
     <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" s="72" t="s">
-        <v>512</v>
-      </c>
-      <c r="C4" s="70" t="s">
+      <c r="A4" s="71" t="s">
         <v>513</v>
       </c>
+      <c r="C4" s="69" t="s">
+        <v>514</v>
+      </c>
     </row>
     <row r="5" ht="15.75" customHeight="1">
-      <c r="A5" s="72" t="s">
-        <v>514</v>
-      </c>
-      <c r="C5" s="70" t="s">
+      <c r="A5" s="71" t="s">
         <v>515</v>
       </c>
+      <c r="C5" s="69" t="s">
+        <v>516</v>
+      </c>
     </row>
     <row r="6" ht="15.75" customHeight="1">
-      <c r="A6" s="69" t="s">
-        <v>516</v>
-      </c>
-      <c r="C6" s="70" t="s">
+      <c r="A6" s="68" t="s">
         <v>517</v>
       </c>
+      <c r="C6" s="69" t="s">
+        <v>518</v>
+      </c>
     </row>
     <row r="7" ht="15.75" customHeight="1">
-      <c r="A7" s="69" t="s">
-        <v>518</v>
-      </c>
-      <c r="C7" s="70" t="s">
+      <c r="A7" s="68" t="s">
         <v>519</v>
       </c>
+      <c r="C7" s="69" t="s">
+        <v>520</v>
+      </c>
     </row>
     <row r="8" ht="15.75" customHeight="1">
-      <c r="A8" s="69" t="s">
-        <v>520</v>
-      </c>
-      <c r="C8" s="70" t="s">
+      <c r="A8" s="68" t="s">
         <v>521</v>
       </c>
+      <c r="C8" s="69" t="s">
+        <v>522</v>
+      </c>
     </row>
     <row r="9" ht="15.75" customHeight="1">
-      <c r="A9" s="69" t="s">
-        <v>522</v>
-      </c>
-      <c r="C9" s="70" t="s">
+      <c r="A9" s="68" t="s">
         <v>523</v>
       </c>
+      <c r="C9" s="69" t="s">
+        <v>524</v>
+      </c>
     </row>
     <row r="10" ht="15.75" customHeight="1">
-      <c r="A10" s="69" t="s">
-        <v>524</v>
-      </c>
-      <c r="C10" s="70" t="s">
+      <c r="A10" s="68" t="s">
         <v>525</v>
       </c>
+      <c r="C10" s="69" t="s">
+        <v>526</v>
+      </c>
     </row>
     <row r="11" ht="15.75" customHeight="1">
-      <c r="A11" s="69" t="s">
-        <v>526</v>
-      </c>
-      <c r="C11" s="70" t="s">
+      <c r="A11" s="68" t="s">
         <v>527</v>
       </c>
+      <c r="C11" s="69" t="s">
+        <v>528</v>
+      </c>
     </row>
     <row r="12" ht="15.75" customHeight="1">
-      <c r="A12" s="69" t="s">
-        <v>528</v>
-      </c>
-      <c r="C12" s="70" t="s">
+      <c r="A12" s="68" t="s">
         <v>529</v>
       </c>
+      <c r="C12" s="69" t="s">
+        <v>530</v>
+      </c>
     </row>
     <row r="13" ht="15.75" customHeight="1">
-      <c r="A13" s="69" t="s">
-        <v>530</v>
-      </c>
-      <c r="C13" s="70" t="s">
+      <c r="A13" s="68" t="s">
         <v>531</v>
       </c>
+      <c r="C13" s="69" t="s">
+        <v>532</v>
+      </c>
     </row>
     <row r="14" ht="15.75" customHeight="1">
-      <c r="A14" s="69" t="s">
-        <v>532</v>
-      </c>
-      <c r="C14" s="70" t="s">
+      <c r="A14" s="68" t="s">
         <v>533</v>
       </c>
+      <c r="C14" s="69" t="s">
+        <v>534</v>
+      </c>
     </row>
     <row r="15" ht="15.75" customHeight="1">
-      <c r="A15" s="69" t="s">
-        <v>534</v>
-      </c>
-      <c r="C15" s="70" t="s">
+      <c r="A15" s="68" t="s">
         <v>535</v>
+      </c>
+      <c r="C15" s="69" t="s">
+        <v>536</v>
       </c>
     </row>
     <row r="16" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
Rebased to remote master branch
</commit_message>
<xml_diff>
--- a/test/excel/Keast_Flatmap_neurolatorNeuron2.xlsx
+++ b/test/excel/Keast_Flatmap_neurolatorNeuron2.xlsx
@@ -11,14 +11,14 @@
     <sheet state="visible" name="nodes" sheetId="6" r:id="rId9"/>
     <sheet state="visible" name="neurons" sheetId="7" r:id="rId10"/>
     <sheet state="visible" name="groups" sheetId="8" r:id="rId11"/>
-    <sheet state="visible" name="publications" sheetId="9" r:id="rId12"/>
+    <sheet state="visible" name="references" sheetId="9" r:id="rId12"/>
     <sheet state="visible" name="localConventions" sheetId="10" r:id="rId13"/>
   </sheets>
   <definedNames/>
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId14" roundtripDataSignature="AMtx7mjJ0E35peh9dp4cCn15t30XOq0sdQ=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId14" roundtripDataSignature="AMtx7mhkddWutpixBXx1M4/nC8P+50n4QA=="/>
     </ext>
   </extLst>
 </workbook>
@@ -133,7 +133,7 @@
   </commentList>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7mioLSU6sDIfqt5Cv2yOX+9s0Zqq9w=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7mhf5vhBr9YH9HwzqnYoeyl9g7+bAw=="/>
     </ext>
   </extLst>
 </comments>
@@ -163,7 +163,7 @@
   </commentList>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7miRXmCpQJk5+aZGYiTk1KAl48YqpA=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7miOmA1jsfzFKailuQPDMkmoaaJn/Q=="/>
     </ext>
   </extLst>
 </comments>
@@ -187,7 +187,7 @@
   </commentList>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7miUyV79QA9KuNn/wvoSUi8UejUCpQ=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7mhctYkkG+oEgCwNF2vzwO72MN3oPQ=="/>
     </ext>
   </extLst>
 </comments>
@@ -220,14 +220,14 @@
   </commentList>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7mjKtv6Q3FyvJtTLXeRVmusOefgsVg=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7mgu/fThSRKvU4TvvJ+L0QCYGpjD2g=="/>
     </ext>
   </extLst>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="706" uniqueCount="562">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="706" uniqueCount="563">
   <si>
     <t>id</t>
   </si>
@@ -491,6 +491,9 @@
     <t>NLX:154731</t>
   </si>
   <si>
+    <t>229bag2</t>
+  </si>
+  <si>
     <t>Segment of neuron  (kblad)</t>
   </si>
   <si>
@@ -755,9 +758,6 @@
     <t>ILX:0777093</t>
   </si>
   <si>
-    <t>k</t>
-  </si>
-  <si>
     <t>K78</t>
   </si>
   <si>
@@ -1728,6 +1728,9 @@
   </si>
   <si>
     <t>groups</t>
+  </si>
+  <si>
+    <t>references</t>
   </si>
   <si>
     <t>neuron-2</t>
@@ -2081,7 +2084,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="74">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -2146,6 +2149,9 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" vertical="bottom"/>
@@ -2223,9 +2229,6 @@
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -2258,14 +2261,11 @@
     <xf borderId="0" fillId="6" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="6" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="6" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
+      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
@@ -3575,106 +3575,106 @@
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="7" t="s">
-        <v>538</v>
-      </c>
-      <c r="B2" s="73" t="s">
         <v>539</v>
+      </c>
+      <c r="B2" s="72" t="s">
+        <v>540</v>
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="7" t="s">
-        <v>540</v>
-      </c>
-      <c r="B3" s="74" t="s">
         <v>541</v>
+      </c>
+      <c r="B3" s="73" t="s">
+        <v>542</v>
       </c>
     </row>
     <row r="4" ht="15.75" customHeight="1">
       <c r="A4" s="7" t="s">
-        <v>542</v>
-      </c>
-      <c r="B4" s="74" t="s">
         <v>543</v>
+      </c>
+      <c r="B4" s="73" t="s">
+        <v>544</v>
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="7" t="s">
-        <v>544</v>
-      </c>
-      <c r="B5" s="74" t="s">
         <v>545</v>
+      </c>
+      <c r="B5" s="73" t="s">
+        <v>546</v>
       </c>
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="7" t="s">
-        <v>546</v>
-      </c>
-      <c r="B6" s="74" t="s">
         <v>547</v>
+      </c>
+      <c r="B6" s="73" t="s">
+        <v>548</v>
       </c>
     </row>
     <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="7" t="s">
-        <v>548</v>
-      </c>
-      <c r="B7" s="74" t="s">
         <v>549</v>
+      </c>
+      <c r="B7" s="73" t="s">
+        <v>550</v>
       </c>
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="7" t="s">
-        <v>550</v>
-      </c>
-      <c r="B8" s="74" t="s">
         <v>551</v>
+      </c>
+      <c r="B8" s="73" t="s">
+        <v>552</v>
       </c>
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="7" t="s">
-        <v>552</v>
-      </c>
-      <c r="B9" s="74" t="s">
         <v>553</v>
+      </c>
+      <c r="B9" s="73" t="s">
+        <v>554</v>
       </c>
     </row>
     <row r="10" ht="15.75" customHeight="1">
       <c r="A10" s="7" t="s">
-        <v>554</v>
-      </c>
-      <c r="B10" s="74" t="s">
         <v>555</v>
+      </c>
+      <c r="B10" s="73" t="s">
+        <v>556</v>
       </c>
     </row>
     <row r="11" ht="15.75" customHeight="1">
       <c r="A11" s="7" t="s">
-        <v>556</v>
-      </c>
-      <c r="B11" s="74" t="s">
         <v>557</v>
+      </c>
+      <c r="B11" s="73" t="s">
+        <v>558</v>
       </c>
     </row>
     <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="2" t="s">
-        <v>558</v>
-      </c>
-      <c r="B12" s="70" t="s">
         <v>559</v>
+      </c>
+      <c r="B12" s="69" t="s">
+        <v>560</v>
       </c>
     </row>
     <row r="13" ht="15.75" customHeight="1">
       <c r="A13" s="2" t="s">
-        <v>560</v>
-      </c>
-      <c r="B13" s="70" t="s">
         <v>561</v>
+      </c>
+      <c r="B13" s="69" t="s">
+        <v>562</v>
       </c>
     </row>
     <row r="14" ht="15.75" customHeight="1"/>
@@ -4698,7 +4698,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="14.57"/>
+    <col customWidth="1" min="1" max="1" width="29.71"/>
     <col customWidth="1" min="2" max="2" width="60.14"/>
     <col customWidth="1" min="3" max="3" width="18.57"/>
     <col customWidth="1" min="4" max="4" width="11.29"/>
@@ -5266,8 +5266,11 @@
       <c r="Q17" s="7"/>
     </row>
     <row r="18" ht="15.75" customHeight="1">
-      <c r="A18" s="7" t="s">
+      <c r="A18" s="23" t="s">
         <v>87</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>88</v>
       </c>
       <c r="C18" s="8" t="s">
         <v>83</v>
@@ -5277,12 +5280,12 @@
         <v>1</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="G18" s="7"/>
       <c r="H18" s="7"/>
       <c r="I18" s="7"/>
-      <c r="J18" s="23">
+      <c r="J18" s="24">
         <v>229.0</v>
       </c>
       <c r="K18" s="7"/>
@@ -5295,7 +5298,7 @@
     </row>
     <row r="19" ht="15.75" customHeight="1">
       <c r="A19" s="11" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B19" s="7" t="s">
         <v>82</v>
@@ -5308,12 +5311,12 @@
         <v>1</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="G19" s="7"/>
       <c r="H19" s="7"/>
       <c r="I19" s="7"/>
-      <c r="J19" s="23">
+      <c r="J19" s="24">
         <v>229.0</v>
       </c>
       <c r="K19" s="7"/>
@@ -5329,7 +5332,7 @@
         <v>64</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C20" s="20" t="s">
         <v>86</v>
@@ -5340,7 +5343,7 @@
       <c r="G20" s="7"/>
       <c r="H20" s="7"/>
       <c r="I20" s="7"/>
-      <c r="J20" s="23">
+      <c r="J20" s="24">
         <v>229.0</v>
       </c>
       <c r="K20" s="7"/>
@@ -5358,7 +5361,7 @@
         <v>39</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C21" s="20" t="s">
         <v>86</v>
@@ -5369,7 +5372,7 @@
       <c r="G21" s="7"/>
       <c r="H21" s="7"/>
       <c r="I21" s="7"/>
-      <c r="J21" s="23">
+      <c r="J21" s="24">
         <v>229.0</v>
       </c>
       <c r="K21" s="7"/>
@@ -5387,7 +5390,7 @@
         <v>43</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C22" s="20" t="s">
         <v>86</v>
@@ -5398,7 +5401,7 @@
       <c r="G22" s="7"/>
       <c r="H22" s="7"/>
       <c r="I22" s="7"/>
-      <c r="J22" s="23">
+      <c r="J22" s="24">
         <v>229.0</v>
       </c>
       <c r="K22" s="7"/>
@@ -5416,7 +5419,7 @@
         <v>52</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C23" s="20" t="s">
         <v>86</v>
@@ -5427,7 +5430,7 @@
       <c r="G23" s="7"/>
       <c r="H23" s="7"/>
       <c r="I23" s="7"/>
-      <c r="J23" s="23">
+      <c r="J23" s="24">
         <v>229.0</v>
       </c>
       <c r="K23" s="7"/>
@@ -5445,7 +5448,7 @@
         <v>56</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C24" s="20" t="s">
         <v>86</v>
@@ -5456,7 +5459,7 @@
       <c r="G24" s="7"/>
       <c r="H24" s="7"/>
       <c r="I24" s="7"/>
-      <c r="J24" s="23">
+      <c r="J24" s="24">
         <v>229.0</v>
       </c>
       <c r="K24" s="7"/>
@@ -5474,7 +5477,7 @@
         <v>60</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C25" s="20" t="s">
         <v>86</v>
@@ -5485,7 +5488,7 @@
       <c r="G25" s="7"/>
       <c r="H25" s="7"/>
       <c r="I25" s="7"/>
-      <c r="J25" s="23">
+      <c r="J25" s="24">
         <v>229.0</v>
       </c>
       <c r="K25" s="7"/>
@@ -5503,7 +5506,7 @@
         <v>71</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C26" s="20" t="s">
         <v>86</v>
@@ -5514,7 +5517,7 @@
       <c r="G26" s="7"/>
       <c r="H26" s="7"/>
       <c r="I26" s="7"/>
-      <c r="J26" s="23">
+      <c r="J26" s="24">
         <v>229.0</v>
       </c>
       <c r="K26" s="7"/>
@@ -5529,13 +5532,13 @@
     </row>
     <row r="27" ht="15.75" customHeight="1">
       <c r="A27" s="11" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D27" s="7"/>
       <c r="E27" s="7"/>
@@ -5554,13 +5557,13 @@
     </row>
     <row r="28" ht="15.75" customHeight="1">
       <c r="A28" s="11" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D28" s="7"/>
       <c r="E28" s="7"/>
@@ -5579,13 +5582,13 @@
     </row>
     <row r="29" ht="15.75" customHeight="1">
       <c r="A29" s="11" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D29" s="7"/>
       <c r="E29" s="7"/>
@@ -5597,7 +5600,7 @@
       <c r="K29" s="7"/>
       <c r="L29" s="11"/>
       <c r="M29" s="11" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="N29" s="11" t="s">
         <v>35</v>
@@ -5608,13 +5611,13 @@
     </row>
     <row r="30" ht="15.75" customHeight="1">
       <c r="A30" s="11" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D30" s="7"/>
       <c r="E30" s="7"/>
@@ -5626,7 +5629,7 @@
       <c r="K30" s="7"/>
       <c r="L30" s="11"/>
       <c r="M30" s="11" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="N30" s="11" t="s">
         <v>35</v>
@@ -5637,13 +5640,13 @@
     </row>
     <row r="31" ht="15.75" customHeight="1">
       <c r="A31" s="11" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D31" s="7"/>
       <c r="E31" s="7"/>
@@ -5662,13 +5665,13 @@
     </row>
     <row r="32" ht="15.75" customHeight="1">
       <c r="A32" s="11" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D32" s="7"/>
       <c r="E32" s="7"/>
@@ -5687,13 +5690,13 @@
     </row>
     <row r="33" ht="15.75" customHeight="1">
       <c r="A33" s="11" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D33" s="7"/>
       <c r="E33" s="7"/>
@@ -5712,13 +5715,13 @@
     </row>
     <row r="34" ht="15.75" customHeight="1">
       <c r="A34" s="11" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D34" s="7"/>
       <c r="E34" s="18"/>
@@ -5730,10 +5733,10 @@
       <c r="K34" s="7"/>
       <c r="L34" s="7"/>
       <c r="M34" s="7" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="N34" s="11" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="O34" s="7"/>
       <c r="P34" s="7"/>
@@ -5741,13 +5744,13 @@
     </row>
     <row r="35" ht="15.75" customHeight="1">
       <c r="A35" s="11" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D35" s="7"/>
       <c r="E35" s="18"/>
@@ -5759,10 +5762,10 @@
       <c r="K35" s="7"/>
       <c r="L35" s="7"/>
       <c r="M35" s="7" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="N35" s="11" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="O35" s="7"/>
       <c r="P35" s="7"/>
@@ -5770,13 +5773,13 @@
     </row>
     <row r="36" ht="15.75" customHeight="1">
       <c r="A36" s="11" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D36" s="7"/>
       <c r="E36" s="7"/>
@@ -5795,13 +5798,13 @@
     </row>
     <row r="37" ht="15.75" customHeight="1">
       <c r="A37" s="11" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D37" s="7"/>
       <c r="E37" s="7"/>
@@ -5820,13 +5823,13 @@
     </row>
     <row r="38" ht="15.75" customHeight="1">
       <c r="A38" s="11" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D38" s="7"/>
       <c r="E38" s="7"/>
@@ -5845,13 +5848,13 @@
     </row>
     <row r="39" ht="15.75" customHeight="1">
       <c r="A39" s="11" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D39" s="7"/>
       <c r="E39" s="7"/>
@@ -5870,13 +5873,13 @@
     </row>
     <row r="40" ht="15.75" customHeight="1">
       <c r="A40" s="11" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C40" s="7" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D40" s="7"/>
       <c r="E40" s="7"/>
@@ -5895,13 +5898,13 @@
     </row>
     <row r="41" ht="15.75" customHeight="1">
       <c r="A41" s="11" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D41" s="7"/>
       <c r="E41" s="7"/>
@@ -5920,13 +5923,13 @@
     </row>
     <row r="42" ht="15.75" customHeight="1">
       <c r="A42" s="11" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C42" s="7" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
@@ -5945,13 +5948,13 @@
     </row>
     <row r="43" ht="15.75" customHeight="1">
       <c r="A43" s="11" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D43" s="7"/>
       <c r="E43" s="7"/>
@@ -5970,13 +5973,13 @@
     </row>
     <row r="44" ht="15.75" customHeight="1">
       <c r="A44" s="11" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C44" s="7" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="D44" s="7"/>
       <c r="E44" s="7"/>
@@ -5995,13 +5998,13 @@
     </row>
     <row r="45" ht="15.75" customHeight="1">
       <c r="A45" s="11" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C45" s="7" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D45" s="7"/>
       <c r="E45" s="7"/>
@@ -6020,13 +6023,13 @@
     </row>
     <row r="46" ht="15.75" customHeight="1">
       <c r="A46" s="11" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B46" s="8" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C46" s="7" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D46" s="7"/>
       <c r="E46" s="7"/>
@@ -6045,13 +6048,13 @@
     </row>
     <row r="47" ht="15.75" customHeight="1">
       <c r="A47" s="11" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C47" s="7" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D47" s="7"/>
       <c r="E47" s="7"/>
@@ -6070,13 +6073,13 @@
     </row>
     <row r="48" ht="15.75" customHeight="1">
       <c r="A48" s="11" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B48" s="8" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C48" s="7" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="D48" s="7"/>
       <c r="E48" s="7"/>
@@ -6095,13 +6098,13 @@
     </row>
     <row r="49" ht="15.75" customHeight="1">
       <c r="A49" s="11" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B49" s="8" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C49" s="7" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D49" s="7"/>
       <c r="E49" s="7"/>
@@ -6120,20 +6123,18 @@
     </row>
     <row r="50" ht="15.75" customHeight="1">
       <c r="A50" s="11" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B50" s="8" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C50" s="7" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="D50" s="7"/>
       <c r="E50" s="7"/>
       <c r="F50" s="7"/>
-      <c r="G50" s="7" t="s">
-        <v>175</v>
-      </c>
+      <c r="G50" s="7"/>
       <c r="H50" s="7"/>
       <c r="I50" s="7"/>
       <c r="J50" s="7"/>
@@ -6192,8 +6193,8 @@
       <c r="I52" s="7"/>
       <c r="J52" s="7"/>
       <c r="K52" s="7"/>
-      <c r="L52" s="24"/>
-      <c r="M52" s="25" t="s">
+      <c r="L52" s="25"/>
+      <c r="M52" s="26" t="s">
         <v>183</v>
       </c>
       <c r="N52" s="11" t="s">
@@ -6255,7 +6256,7 @@
         <v>191</v>
       </c>
       <c r="N54" s="11" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="O54" s="7"/>
       <c r="P54" s="7"/>
@@ -6717,7 +6718,7 @@
       <c r="F72" s="7"/>
       <c r="G72" s="7"/>
       <c r="H72" s="7"/>
-      <c r="I72" s="26" t="s">
+      <c r="I72" s="27" t="s">
         <v>250</v>
       </c>
       <c r="J72" s="7"/>
@@ -6748,7 +6749,7 @@
       <c r="F73" s="7"/>
       <c r="G73" s="7"/>
       <c r="H73" s="7"/>
-      <c r="I73" s="26" t="s">
+      <c r="I73" s="27" t="s">
         <v>250</v>
       </c>
       <c r="J73" s="7"/>
@@ -6779,7 +6780,7 @@
       <c r="F74" s="7"/>
       <c r="G74" s="7"/>
       <c r="H74" s="7"/>
-      <c r="I74" s="26" t="s">
+      <c r="I74" s="27" t="s">
         <v>260</v>
       </c>
       <c r="J74" s="7"/>
@@ -6792,33 +6793,33 @@
       <c r="Q74" s="7"/>
     </row>
     <row r="75" ht="15.75" customHeight="1">
-      <c r="A75" s="27" t="s">
+      <c r="A75" s="28" t="s">
         <v>261</v>
       </c>
-      <c r="B75" s="28" t="s">
+      <c r="B75" s="29" t="s">
         <v>262</v>
       </c>
-      <c r="C75" s="28" t="s">
+      <c r="C75" s="29" t="s">
         <v>263</v>
       </c>
-      <c r="D75" s="28"/>
-      <c r="E75" s="28"/>
-      <c r="F75" s="28"/>
-      <c r="G75" s="28"/>
-      <c r="H75" s="28"/>
-      <c r="I75" s="28"/>
-      <c r="J75" s="28"/>
-      <c r="K75" s="28"/>
-      <c r="L75" s="28"/>
-      <c r="M75" s="28" t="s">
+      <c r="D75" s="29"/>
+      <c r="E75" s="29"/>
+      <c r="F75" s="29"/>
+      <c r="G75" s="29"/>
+      <c r="H75" s="29"/>
+      <c r="I75" s="29"/>
+      <c r="J75" s="29"/>
+      <c r="K75" s="29"/>
+      <c r="L75" s="29"/>
+      <c r="M75" s="29" t="s">
         <v>264</v>
       </c>
-      <c r="N75" s="27" t="s">
+      <c r="N75" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="O75" s="28"/>
-      <c r="P75" s="28"/>
-      <c r="Q75" s="28"/>
+      <c r="O75" s="29"/>
+      <c r="P75" s="29"/>
+      <c r="Q75" s="29"/>
     </row>
     <row r="76" ht="15.75" customHeight="1">
       <c r="A76" s="11" t="s">
@@ -6837,7 +6838,7 @@
       <c r="F76" s="7"/>
       <c r="G76" s="7"/>
       <c r="H76" s="7"/>
-      <c r="I76" s="26" t="s">
+      <c r="I76" s="27" t="s">
         <v>268</v>
       </c>
       <c r="J76" s="7"/>
@@ -6853,7 +6854,7 @@
       <c r="A77" s="11" t="s">
         <v>269</v>
       </c>
-      <c r="B77" s="29" t="s">
+      <c r="B77" s="30" t="s">
         <v>270</v>
       </c>
       <c r="C77" s="7" t="s">
@@ -6868,11 +6869,11 @@
       <c r="J77" s="7"/>
       <c r="K77" s="7"/>
       <c r="L77" s="7"/>
-      <c r="M77" s="30" t="s">
+      <c r="M77" s="31" t="s">
         <v>272</v>
       </c>
       <c r="N77" s="11" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="O77" s="7"/>
       <c r="P77" s="7"/>
@@ -6942,7 +6943,7 @@
       <c r="G80" s="7"/>
       <c r="H80" s="7"/>
       <c r="I80" s="7"/>
-      <c r="J80" s="23">
+      <c r="J80" s="24">
         <v>229.0</v>
       </c>
       <c r="K80" s="7"/>
@@ -6969,7 +6970,7 @@
       <c r="G81" s="7"/>
       <c r="H81" s="7"/>
       <c r="I81" s="7"/>
-      <c r="J81" s="23">
+      <c r="J81" s="24">
         <v>229.0</v>
       </c>
       <c r="K81" s="7"/>
@@ -6998,7 +6999,7 @@
       <c r="G82" s="7"/>
       <c r="H82" s="7"/>
       <c r="I82" s="7"/>
-      <c r="J82" s="23">
+      <c r="J82" s="24">
         <v>229.0</v>
       </c>
       <c r="K82" s="7"/>
@@ -7054,8 +7055,8 @@
       <c r="I84" s="7"/>
       <c r="J84" s="7"/>
       <c r="K84" s="7"/>
-      <c r="L84" s="31"/>
-      <c r="M84" s="31"/>
+      <c r="L84" s="32"/>
+      <c r="M84" s="32"/>
       <c r="N84" s="11"/>
       <c r="O84" s="7"/>
       <c r="P84" s="7"/>
@@ -7112,138 +7113,138 @@
       <c r="Q86" s="7"/>
     </row>
     <row r="87" ht="15.75" customHeight="1">
-      <c r="A87" s="32" t="s">
+      <c r="A87" s="33" t="s">
         <v>292</v>
       </c>
-      <c r="B87" s="33" t="s">
+      <c r="B87" s="34" t="s">
         <v>293</v>
       </c>
-      <c r="C87" s="34" t="s">
+      <c r="C87" s="35" t="s">
         <v>86</v>
       </c>
-      <c r="D87" s="33"/>
-      <c r="E87" s="35"/>
-      <c r="F87" s="33"/>
-      <c r="G87" s="33"/>
-      <c r="H87" s="33"/>
-      <c r="I87" s="33"/>
-      <c r="J87" s="36">
+      <c r="D87" s="34"/>
+      <c r="E87" s="36"/>
+      <c r="F87" s="34"/>
+      <c r="G87" s="34"/>
+      <c r="H87" s="34"/>
+      <c r="I87" s="34"/>
+      <c r="J87" s="37">
         <v>229.0</v>
       </c>
-      <c r="K87" s="33"/>
-      <c r="L87" s="33" t="s">
-        <v>121</v>
-      </c>
-      <c r="M87" s="33"/>
-      <c r="N87" s="32"/>
-      <c r="O87" s="33"/>
-      <c r="P87" s="33"/>
-      <c r="Q87" s="33"/>
+      <c r="K87" s="34"/>
+      <c r="L87" s="34" t="s">
+        <v>122</v>
+      </c>
+      <c r="M87" s="34"/>
+      <c r="N87" s="33"/>
+      <c r="O87" s="34"/>
+      <c r="P87" s="34"/>
+      <c r="Q87" s="34"/>
     </row>
     <row r="88" ht="15.75" customHeight="1">
-      <c r="A88" s="32" t="s">
+      <c r="A88" s="33" t="s">
         <v>294</v>
       </c>
-      <c r="B88" s="33" t="s">
+      <c r="B88" s="34" t="s">
         <v>295</v>
       </c>
-      <c r="C88" s="34" t="s">
+      <c r="C88" s="35" t="s">
         <v>86</v>
       </c>
-      <c r="D88" s="33"/>
-      <c r="E88" s="33"/>
-      <c r="F88" s="33"/>
-      <c r="G88" s="33"/>
-      <c r="H88" s="33"/>
-      <c r="I88" s="33"/>
-      <c r="J88" s="36">
+      <c r="D88" s="34"/>
+      <c r="E88" s="34"/>
+      <c r="F88" s="34"/>
+      <c r="G88" s="34"/>
+      <c r="H88" s="34"/>
+      <c r="I88" s="34"/>
+      <c r="J88" s="37">
         <v>229.0</v>
       </c>
-      <c r="K88" s="33"/>
-      <c r="L88" s="33" t="s">
-        <v>126</v>
-      </c>
-      <c r="M88" s="33"/>
-      <c r="N88" s="32"/>
-      <c r="O88" s="33"/>
-      <c r="P88" s="33"/>
-      <c r="Q88" s="33"/>
+      <c r="K88" s="34"/>
+      <c r="L88" s="34" t="s">
+        <v>127</v>
+      </c>
+      <c r="M88" s="34"/>
+      <c r="N88" s="33"/>
+      <c r="O88" s="34"/>
+      <c r="P88" s="34"/>
+      <c r="Q88" s="34"/>
     </row>
     <row r="89" ht="15.75" customHeight="1">
-      <c r="A89" s="32" t="s">
+      <c r="A89" s="33" t="s">
         <v>296</v>
       </c>
-      <c r="B89" s="33" t="s">
+      <c r="B89" s="34" t="s">
         <v>297</v>
       </c>
-      <c r="C89" s="34" t="s">
+      <c r="C89" s="35" t="s">
         <v>86</v>
       </c>
-      <c r="D89" s="33"/>
-      <c r="E89" s="35"/>
-      <c r="F89" s="33"/>
-      <c r="G89" s="33"/>
-      <c r="H89" s="33"/>
-      <c r="I89" s="33"/>
-      <c r="J89" s="36">
+      <c r="D89" s="34"/>
+      <c r="E89" s="36"/>
+      <c r="F89" s="34"/>
+      <c r="G89" s="34"/>
+      <c r="H89" s="34"/>
+      <c r="I89" s="34"/>
+      <c r="J89" s="37">
         <v>229.0</v>
       </c>
-      <c r="K89" s="33"/>
-      <c r="L89" s="32" t="s">
-        <v>121</v>
-      </c>
-      <c r="M89" s="32"/>
-      <c r="N89" s="32"/>
-      <c r="O89" s="33"/>
-      <c r="P89" s="33"/>
-      <c r="Q89" s="33"/>
+      <c r="K89" s="34"/>
+      <c r="L89" s="33" t="s">
+        <v>122</v>
+      </c>
+      <c r="M89" s="33"/>
+      <c r="N89" s="33"/>
+      <c r="O89" s="34"/>
+      <c r="P89" s="34"/>
+      <c r="Q89" s="34"/>
     </row>
     <row r="90" ht="15.75" customHeight="1">
-      <c r="A90" s="32" t="s">
+      <c r="A90" s="33" t="s">
         <v>298</v>
       </c>
-      <c r="B90" s="33" t="s">
+      <c r="B90" s="34" t="s">
         <v>299</v>
       </c>
-      <c r="C90" s="34" t="s">
+      <c r="C90" s="35" t="s">
         <v>86</v>
       </c>
-      <c r="D90" s="33"/>
-      <c r="E90" s="35"/>
-      <c r="F90" s="33"/>
-      <c r="G90" s="33"/>
-      <c r="H90" s="33"/>
-      <c r="I90" s="33"/>
-      <c r="J90" s="36">
+      <c r="D90" s="34"/>
+      <c r="E90" s="36"/>
+      <c r="F90" s="34"/>
+      <c r="G90" s="34"/>
+      <c r="H90" s="34"/>
+      <c r="I90" s="34"/>
+      <c r="J90" s="37">
         <v>229.0</v>
       </c>
-      <c r="K90" s="33"/>
-      <c r="L90" s="32" t="s">
-        <v>126</v>
-      </c>
-      <c r="M90" s="32"/>
-      <c r="N90" s="32"/>
-      <c r="O90" s="33"/>
-      <c r="P90" s="33"/>
-      <c r="Q90" s="33"/>
+      <c r="K90" s="34"/>
+      <c r="L90" s="33" t="s">
+        <v>127</v>
+      </c>
+      <c r="M90" s="33"/>
+      <c r="N90" s="33"/>
+      <c r="O90" s="34"/>
+      <c r="P90" s="34"/>
+      <c r="Q90" s="34"/>
     </row>
     <row r="91" ht="15.75" customHeight="1">
-      <c r="A91" s="37" t="s">
+      <c r="A91" s="38" t="s">
         <v>300</v>
       </c>
-      <c r="B91" s="38" t="s">
+      <c r="B91" s="39" t="s">
         <v>301</v>
       </c>
-      <c r="C91" s="38" t="s">
+      <c r="C91" s="39" t="s">
         <v>302</v>
       </c>
-      <c r="D91" s="38"/>
-      <c r="E91" s="38"/>
-      <c r="F91" s="38"/>
-      <c r="G91" s="38"/>
-      <c r="H91" s="38"/>
-      <c r="I91" s="38"/>
-      <c r="J91" s="38"/>
+      <c r="D91" s="39"/>
+      <c r="E91" s="39"/>
+      <c r="F91" s="39"/>
+      <c r="G91" s="39"/>
+      <c r="H91" s="39"/>
+      <c r="I91" s="39"/>
+      <c r="J91" s="39"/>
       <c r="K91" s="11"/>
       <c r="L91" s="11"/>
       <c r="M91" s="11" t="s">
@@ -7257,62 +7258,62 @@
       <c r="Q91" s="7"/>
     </row>
     <row r="92" ht="15.75" customHeight="1">
-      <c r="A92" s="32" t="s">
-        <v>107</v>
-      </c>
-      <c r="B92" s="33" t="s">
+      <c r="A92" s="33" t="s">
+        <v>108</v>
+      </c>
+      <c r="B92" s="34" t="s">
         <v>304</v>
       </c>
-      <c r="C92" s="34" t="s">
+      <c r="C92" s="35" t="s">
         <v>86</v>
       </c>
-      <c r="D92" s="33"/>
-      <c r="E92" s="33"/>
-      <c r="F92" s="33"/>
-      <c r="G92" s="33"/>
-      <c r="H92" s="33"/>
-      <c r="I92" s="33"/>
-      <c r="J92" s="36">
+      <c r="D92" s="34"/>
+      <c r="E92" s="34"/>
+      <c r="F92" s="34"/>
+      <c r="G92" s="34"/>
+      <c r="H92" s="34"/>
+      <c r="I92" s="34"/>
+      <c r="J92" s="37">
         <v>229.0</v>
       </c>
-      <c r="K92" s="33"/>
-      <c r="L92" s="33" t="s">
-        <v>104</v>
-      </c>
-      <c r="M92" s="33"/>
-      <c r="N92" s="32"/>
-      <c r="O92" s="33"/>
-      <c r="P92" s="33"/>
-      <c r="Q92" s="33"/>
+      <c r="K92" s="34"/>
+      <c r="L92" s="34" t="s">
+        <v>105</v>
+      </c>
+      <c r="M92" s="34"/>
+      <c r="N92" s="33"/>
+      <c r="O92" s="34"/>
+      <c r="P92" s="34"/>
+      <c r="Q92" s="34"/>
     </row>
     <row r="93" ht="15.75" customHeight="1">
-      <c r="A93" s="32" t="s">
-        <v>111</v>
-      </c>
-      <c r="B93" s="33" t="s">
+      <c r="A93" s="33" t="s">
+        <v>112</v>
+      </c>
+      <c r="B93" s="34" t="s">
         <v>305</v>
       </c>
-      <c r="C93" s="33" t="s">
+      <c r="C93" s="34" t="s">
         <v>306</v>
       </c>
-      <c r="D93" s="33"/>
-      <c r="E93" s="33"/>
-      <c r="F93" s="33"/>
-      <c r="G93" s="33"/>
-      <c r="H93" s="33"/>
-      <c r="I93" s="33"/>
-      <c r="J93" s="36">
+      <c r="D93" s="34"/>
+      <c r="E93" s="34"/>
+      <c r="F93" s="34"/>
+      <c r="G93" s="34"/>
+      <c r="H93" s="34"/>
+      <c r="I93" s="34"/>
+      <c r="J93" s="37">
         <v>229.0</v>
       </c>
-      <c r="K93" s="33"/>
-      <c r="L93" s="33" t="s">
-        <v>108</v>
-      </c>
-      <c r="M93" s="33"/>
-      <c r="N93" s="32"/>
-      <c r="O93" s="33"/>
-      <c r="P93" s="33"/>
-      <c r="Q93" s="33"/>
+      <c r="K93" s="34"/>
+      <c r="L93" s="34" t="s">
+        <v>109</v>
+      </c>
+      <c r="M93" s="34"/>
+      <c r="N93" s="33"/>
+      <c r="O93" s="34"/>
+      <c r="P93" s="34"/>
+      <c r="Q93" s="34"/>
     </row>
     <row r="94" ht="15.75" customHeight="1"/>
     <row r="95" ht="15.75" customHeight="1"/>
@@ -8191,16 +8192,16 @@
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="39" t="s">
+      <c r="B1" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="39" t="s">
+      <c r="C1" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="39" t="s">
+      <c r="D1" s="40" t="s">
         <v>12</v>
       </c>
     </row>
@@ -8276,7 +8277,7 @@
       <c r="C7" s="8" t="s">
         <v>325</v>
       </c>
-      <c r="D7" s="40" t="s">
+      <c r="D7" s="41" t="s">
         <v>326</v>
       </c>
     </row>
@@ -8290,7 +8291,7 @@
       <c r="C8" s="8" t="s">
         <v>309</v>
       </c>
-      <c r="D8" s="40" t="s">
+      <c r="D8" s="41" t="s">
         <v>326</v>
       </c>
     </row>
@@ -8304,7 +8305,7 @@
       <c r="C9" s="8" t="s">
         <v>330</v>
       </c>
-      <c r="D9" s="41" t="s">
+      <c r="D9" s="42" t="s">
         <v>331</v>
       </c>
     </row>
@@ -8318,7 +8319,7 @@
       <c r="C10" s="8" t="s">
         <v>334</v>
       </c>
-      <c r="D10" s="40" t="s">
+      <c r="D10" s="41" t="s">
         <v>326</v>
       </c>
     </row>
@@ -8332,19 +8333,19 @@
       <c r="C11" s="8" t="s">
         <v>337</v>
       </c>
-      <c r="D11" s="40"/>
+      <c r="D11" s="41"/>
     </row>
     <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="14" t="s">
         <v>338</v>
       </c>
-      <c r="B12" s="40" t="s">
+      <c r="B12" s="41" t="s">
         <v>339</v>
       </c>
-      <c r="C12" s="40" t="s">
+      <c r="C12" s="41" t="s">
         <v>340</v>
       </c>
-      <c r="D12" s="40"/>
+      <c r="D12" s="41"/>
     </row>
     <row r="13" ht="15.75" customHeight="1">
       <c r="A13" s="14" t="s">
@@ -8353,10 +8354,10 @@
       <c r="B13" s="8" t="s">
         <v>342</v>
       </c>
-      <c r="C13" s="40" t="s">
+      <c r="C13" s="41" t="s">
         <v>343</v>
       </c>
-      <c r="D13" s="40"/>
+      <c r="D13" s="41"/>
     </row>
     <row r="14" ht="15.75" customHeight="1">
       <c r="A14" s="14" t="s">
@@ -8365,10 +8366,10 @@
       <c r="B14" s="8" t="s">
         <v>345</v>
       </c>
-      <c r="C14" s="40" t="s">
+      <c r="C14" s="41" t="s">
         <v>346</v>
       </c>
-      <c r="D14" s="40"/>
+      <c r="D14" s="41"/>
     </row>
     <row r="15" ht="15.75" customHeight="1">
       <c r="A15" s="14" t="s">
@@ -8377,10 +8378,10 @@
       <c r="B15" s="8" t="s">
         <v>348</v>
       </c>
-      <c r="C15" s="40" t="s">
+      <c r="C15" s="41" t="s">
         <v>349</v>
       </c>
-      <c r="D15" s="40"/>
+      <c r="D15" s="41"/>
     </row>
     <row r="16" ht="15.75" customHeight="1">
       <c r="A16" s="14" t="s">
@@ -8389,10 +8390,10 @@
       <c r="B16" s="8" t="s">
         <v>351</v>
       </c>
-      <c r="C16" s="40" t="s">
+      <c r="C16" s="41" t="s">
         <v>352</v>
       </c>
-      <c r="D16" s="40"/>
+      <c r="D16" s="41"/>
     </row>
     <row r="17" ht="15.75" customHeight="1">
       <c r="A17" s="14" t="s">
@@ -8401,10 +8402,10 @@
       <c r="B17" s="8" t="s">
         <v>354</v>
       </c>
-      <c r="C17" s="40" t="s">
+      <c r="C17" s="41" t="s">
         <v>355</v>
       </c>
-      <c r="D17" s="40"/>
+      <c r="D17" s="41"/>
     </row>
     <row r="18" ht="15.75" customHeight="1">
       <c r="A18" s="14" t="s">
@@ -8413,10 +8414,10 @@
       <c r="B18" s="8" t="s">
         <v>357</v>
       </c>
-      <c r="C18" s="40" t="s">
+      <c r="C18" s="41" t="s">
         <v>358</v>
       </c>
-      <c r="D18" s="40"/>
+      <c r="D18" s="41"/>
     </row>
     <row r="19" ht="15.75" customHeight="1">
       <c r="A19" s="14" t="s">
@@ -8425,10 +8426,10 @@
       <c r="B19" s="8" t="s">
         <v>360</v>
       </c>
-      <c r="C19" s="40" t="s">
+      <c r="C19" s="41" t="s">
         <v>361</v>
       </c>
-      <c r="D19" s="40"/>
+      <c r="D19" s="41"/>
     </row>
     <row r="20" ht="15.75" customHeight="1">
       <c r="A20" s="14" t="s">
@@ -8437,10 +8438,10 @@
       <c r="B20" s="8" t="s">
         <v>363</v>
       </c>
-      <c r="C20" s="42" t="s">
+      <c r="C20" s="43" t="s">
         <v>330</v>
       </c>
-      <c r="D20" s="40"/>
+      <c r="D20" s="41"/>
     </row>
     <row r="21" ht="15.75" customHeight="1">
       <c r="A21" s="14" t="s">
@@ -8449,10 +8450,10 @@
       <c r="B21" s="8" t="s">
         <v>365</v>
       </c>
-      <c r="C21" s="42" t="s">
+      <c r="C21" s="43" t="s">
         <v>366</v>
       </c>
-      <c r="D21" s="40"/>
+      <c r="D21" s="41"/>
     </row>
     <row r="22" ht="15.75" customHeight="1">
       <c r="A22" s="14" t="s">
@@ -8461,10 +8462,10 @@
       <c r="B22" s="8" t="s">
         <v>368</v>
       </c>
-      <c r="C22" s="43" t="s">
+      <c r="C22" s="44" t="s">
         <v>369</v>
       </c>
-      <c r="D22" s="40" t="s">
+      <c r="D22" s="41" t="s">
         <v>320</v>
       </c>
     </row>
@@ -8475,10 +8476,10 @@
       <c r="B23" s="7" t="s">
         <v>371</v>
       </c>
-      <c r="C23" s="44" t="s">
+      <c r="C23" s="45" t="s">
         <v>372</v>
       </c>
-      <c r="D23" s="40"/>
+      <c r="D23" s="41"/>
     </row>
     <row r="24" ht="15.75" customHeight="1">
       <c r="A24" s="14" t="s">
@@ -8487,10 +8488,10 @@
       <c r="B24" s="7" t="s">
         <v>374</v>
       </c>
-      <c r="C24" s="44" t="s">
+      <c r="C24" s="45" t="s">
         <v>375</v>
       </c>
-      <c r="D24" s="40"/>
+      <c r="D24" s="41"/>
     </row>
     <row r="25" ht="15.75" customHeight="1">
       <c r="A25" s="14" t="s">
@@ -8499,10 +8500,10 @@
       <c r="B25" s="7" t="s">
         <v>377</v>
       </c>
-      <c r="C25" s="44" t="s">
+      <c r="C25" s="45" t="s">
         <v>378</v>
       </c>
-      <c r="D25" s="40" t="s">
+      <c r="D25" s="41" t="s">
         <v>320</v>
       </c>
     </row>
@@ -8510,13 +8511,13 @@
       <c r="A26" s="14" t="s">
         <v>379</v>
       </c>
-      <c r="B26" s="40" t="s">
+      <c r="B26" s="41" t="s">
         <v>380</v>
       </c>
-      <c r="C26" s="40" t="s">
+      <c r="C26" s="41" t="s">
         <v>381</v>
       </c>
-      <c r="D26" s="40" t="s">
+      <c r="D26" s="41" t="s">
         <v>338</v>
       </c>
     </row>
@@ -8524,229 +8525,229 @@
       <c r="A27" s="14" t="s">
         <v>382</v>
       </c>
-      <c r="B27" s="40" t="s">
+      <c r="B27" s="41" t="s">
         <v>383</v>
       </c>
-      <c r="C27" s="40" t="s">
+      <c r="C27" s="41" t="s">
         <v>384</v>
       </c>
-      <c r="D27" s="40"/>
+      <c r="D27" s="41"/>
     </row>
     <row r="28" ht="15.75" customHeight="1">
       <c r="A28" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="B28" s="40" t="s">
+      <c r="B28" s="41" t="s">
         <v>385</v>
       </c>
-      <c r="C28" s="40" t="s">
+      <c r="C28" s="41" t="s">
         <v>386</v>
       </c>
-      <c r="D28" s="40"/>
+      <c r="D28" s="41"/>
     </row>
     <row r="29" ht="15.75" customHeight="1">
-      <c r="A29" s="29" t="s">
+      <c r="A29" s="30" t="s">
         <v>387</v>
       </c>
       <c r="B29" s="15" t="s">
         <v>388</v>
       </c>
-      <c r="C29" s="29" t="s">
+      <c r="C29" s="30" t="s">
         <v>389</v>
       </c>
-      <c r="D29" s="29"/>
+      <c r="D29" s="30"/>
     </row>
     <row r="30" ht="15.75" customHeight="1">
-      <c r="A30" s="29" t="s">
+      <c r="A30" s="30" t="s">
         <v>390</v>
       </c>
       <c r="B30" s="15" t="s">
         <v>391</v>
       </c>
-      <c r="C30" s="29" t="s">
+      <c r="C30" s="30" t="s">
         <v>392</v>
       </c>
-      <c r="D30" s="29"/>
+      <c r="D30" s="30"/>
     </row>
     <row r="31" ht="15.75" customHeight="1">
-      <c r="A31" s="29" t="s">
+      <c r="A31" s="30" t="s">
         <v>393</v>
       </c>
       <c r="B31" s="15" t="s">
         <v>394</v>
       </c>
-      <c r="C31" s="29" t="s">
+      <c r="C31" s="30" t="s">
         <v>395</v>
       </c>
-      <c r="D31" s="29"/>
+      <c r="D31" s="30"/>
     </row>
     <row r="32" ht="15.75" customHeight="1">
-      <c r="A32" s="29" t="s">
+      <c r="A32" s="30" t="s">
         <v>396</v>
       </c>
       <c r="B32" s="15" t="s">
         <v>397</v>
       </c>
-      <c r="C32" s="29" t="s">
+      <c r="C32" s="30" t="s">
         <v>398</v>
       </c>
-      <c r="D32" s="29"/>
+      <c r="D32" s="30"/>
     </row>
     <row r="33" ht="15.75" customHeight="1">
-      <c r="A33" s="29" t="s">
+      <c r="A33" s="30" t="s">
         <v>399</v>
       </c>
       <c r="B33" s="15" t="s">
         <v>400</v>
       </c>
-      <c r="C33" s="29" t="s">
+      <c r="C33" s="30" t="s">
         <v>401</v>
       </c>
-      <c r="D33" s="29"/>
+      <c r="D33" s="30"/>
     </row>
     <row r="34" ht="15.75" customHeight="1">
-      <c r="A34" s="29" t="s">
+      <c r="A34" s="30" t="s">
         <v>402</v>
       </c>
       <c r="B34" s="15" t="s">
         <v>403</v>
       </c>
-      <c r="C34" s="29" t="s">
+      <c r="C34" s="30" t="s">
         <v>404</v>
       </c>
-      <c r="D34" s="29"/>
+      <c r="D34" s="30"/>
     </row>
     <row r="35" ht="15.75" customHeight="1">
-      <c r="A35" s="29" t="s">
+      <c r="A35" s="30" t="s">
         <v>405</v>
       </c>
       <c r="B35" s="15" t="s">
         <v>406</v>
       </c>
-      <c r="C35" s="29" t="s">
+      <c r="C35" s="30" t="s">
         <v>407</v>
       </c>
-      <c r="D35" s="29"/>
+      <c r="D35" s="30"/>
     </row>
     <row r="36" ht="15.75" customHeight="1">
-      <c r="A36" s="29" t="s">
+      <c r="A36" s="30" t="s">
         <v>408</v>
       </c>
       <c r="B36" s="15" t="s">
         <v>409</v>
       </c>
-      <c r="C36" s="29" t="s">
+      <c r="C36" s="30" t="s">
         <v>410</v>
       </c>
-      <c r="D36" s="29"/>
+      <c r="D36" s="30"/>
     </row>
     <row r="37" ht="15.75" customHeight="1">
-      <c r="A37" s="29" t="s">
+      <c r="A37" s="30" t="s">
         <v>411</v>
       </c>
       <c r="B37" s="15" t="s">
         <v>412</v>
       </c>
-      <c r="C37" s="29" t="s">
+      <c r="C37" s="30" t="s">
         <v>413</v>
       </c>
-      <c r="D37" s="29"/>
+      <c r="D37" s="30"/>
     </row>
     <row r="38" ht="15.75" customHeight="1">
-      <c r="A38" s="29" t="s">
+      <c r="A38" s="30" t="s">
         <v>414</v>
       </c>
       <c r="B38" s="15" t="s">
         <v>415</v>
       </c>
-      <c r="C38" s="29" t="s">
+      <c r="C38" s="30" t="s">
         <v>416</v>
       </c>
-      <c r="D38" s="29"/>
+      <c r="D38" s="30"/>
     </row>
     <row r="39" ht="15.75" customHeight="1">
-      <c r="A39" s="23">
+      <c r="A39" s="24">
         <v>54.0</v>
       </c>
       <c r="B39" s="7" t="s">
         <v>417</v>
       </c>
-      <c r="C39" s="45" t="s">
+      <c r="C39" s="46" t="s">
         <v>418</v>
       </c>
-      <c r="D39" s="23"/>
+      <c r="D39" s="24"/>
     </row>
     <row r="40" ht="15.75" customHeight="1">
-      <c r="A40" s="23">
+      <c r="A40" s="24">
         <v>55.0</v>
       </c>
       <c r="B40" s="7" t="s">
         <v>419</v>
       </c>
-      <c r="C40" s="45" t="s">
+      <c r="C40" s="46" t="s">
         <v>420</v>
       </c>
       <c r="D40" s="7"/>
     </row>
     <row r="41" ht="15.75" customHeight="1">
-      <c r="A41" s="23">
+      <c r="A41" s="24">
         <v>56.0</v>
       </c>
       <c r="B41" s="7" t="s">
         <v>421</v>
       </c>
-      <c r="C41" s="45" t="s">
+      <c r="C41" s="46" t="s">
         <v>422</v>
       </c>
-      <c r="D41" s="23"/>
+      <c r="D41" s="24"/>
     </row>
     <row r="42" ht="15.75" customHeight="1">
-      <c r="A42" s="23">
+      <c r="A42" s="24">
         <v>116.0</v>
       </c>
       <c r="B42" s="7" t="s">
         <v>321</v>
       </c>
-      <c r="C42" s="46" t="s">
+      <c r="C42" s="47" t="s">
         <v>423</v>
       </c>
-      <c r="D42" s="40"/>
+      <c r="D42" s="41"/>
     </row>
     <row r="43" ht="15.75" customHeight="1">
-      <c r="A43" s="23" t="s">
+      <c r="A43" s="24" t="s">
         <v>424</v>
       </c>
       <c r="B43" s="7" t="s">
         <v>425</v>
       </c>
-      <c r="C43" s="46" t="s">
+      <c r="C43" s="47" t="s">
         <v>426</v>
       </c>
-      <c r="D43" s="40"/>
+      <c r="D43" s="41"/>
     </row>
     <row r="44" ht="15.75" customHeight="1">
-      <c r="A44" s="23" t="s">
+      <c r="A44" s="24" t="s">
         <v>427</v>
       </c>
       <c r="B44" s="7" t="s">
         <v>428</v>
       </c>
-      <c r="C44" s="46" t="s">
+      <c r="C44" s="47" t="s">
         <v>429</v>
       </c>
-      <c r="D44" s="40"/>
+      <c r="D44" s="41"/>
     </row>
     <row r="45" ht="15.75" customHeight="1">
-      <c r="A45" s="23" t="s">
+      <c r="A45" s="24" t="s">
         <v>430</v>
       </c>
       <c r="B45" s="7" t="s">
         <v>431</v>
       </c>
-      <c r="C45" s="47" t="s">
+      <c r="C45" s="48" t="s">
         <v>432</v>
       </c>
-      <c r="D45" s="40"/>
+      <c r="D45" s="41"/>
     </row>
     <row r="46" ht="15.75" customHeight="1"/>
     <row r="47" ht="15.75" customHeight="1"/>
@@ -9762,7 +9763,7 @@
       <c r="E2" s="11" t="s">
         <v>277</v>
       </c>
-      <c r="F2" s="23">
+      <c r="F2" s="24">
         <v>4.0</v>
       </c>
       <c r="G2" s="7"/>
@@ -10781,7 +10782,7 @@
       <c r="D1" s="4" t="s">
         <v>440</v>
       </c>
-      <c r="E1" s="48" t="s">
+      <c r="E1" s="49" t="s">
         <v>441</v>
       </c>
       <c r="F1" s="4" t="s">
@@ -10796,10 +10797,10 @@
       <c r="I1" s="4" t="s">
         <v>444</v>
       </c>
-      <c r="J1" s="49" t="s">
+      <c r="J1" s="50" t="s">
         <v>445</v>
       </c>
-      <c r="K1" s="50" t="s">
+      <c r="K1" s="51" t="s">
         <v>446</v>
       </c>
       <c r="L1" s="51" t="s">
@@ -10808,7 +10809,7 @@
       <c r="M1" s="52" t="s">
         <v>448</v>
       </c>
-      <c r="N1" s="31" t="s">
+      <c r="N1" s="32" t="s">
         <v>436</v>
       </c>
     </row>
@@ -10824,7 +10825,7 @@
       </c>
       <c r="D2" s="21"/>
       <c r="E2" s="55" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="F2" s="21" t="s">
         <v>438</v>
@@ -10843,31 +10844,31 @@
       <c r="N2" s="58"/>
     </row>
     <row r="3" ht="15.75" customHeight="1">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="33" t="s">
         <v>452</v>
       </c>
-      <c r="B3" s="33" t="s">
+      <c r="B3" s="34" t="s">
         <v>453</v>
       </c>
       <c r="C3" s="20" t="s">
         <v>454</v>
       </c>
-      <c r="D3" s="33"/>
+      <c r="D3" s="34"/>
       <c r="E3" s="59" t="s">
         <v>81</v>
       </c>
-      <c r="F3" s="33" t="s">
+      <c r="F3" s="34" t="s">
         <v>439</v>
       </c>
-      <c r="G3" s="32" t="s">
+      <c r="G3" s="33" t="s">
         <v>455</v>
       </c>
-      <c r="H3" s="33"/>
-      <c r="I3" s="33"/>
-      <c r="J3" s="33"/>
-      <c r="K3" s="36"/>
-      <c r="L3" s="36" t="s">
-        <v>125</v>
+      <c r="H3" s="34"/>
+      <c r="I3" s="34"/>
+      <c r="J3" s="34"/>
+      <c r="K3" s="37"/>
+      <c r="L3" s="37" t="s">
+        <v>126</v>
       </c>
       <c r="M3" s="60" t="s">
         <v>456</v>
@@ -10875,65 +10876,65 @@
       <c r="N3" s="61"/>
     </row>
     <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" s="32" t="s">
+      <c r="A4" s="33" t="s">
         <v>457</v>
       </c>
-      <c r="B4" s="33" t="s">
+      <c r="B4" s="34" t="s">
         <v>458</v>
       </c>
       <c r="C4" s="20" t="s">
         <v>454</v>
       </c>
-      <c r="D4" s="33"/>
+      <c r="D4" s="34"/>
       <c r="E4" s="59" t="s">
-        <v>89</v>
-      </c>
-      <c r="F4" s="33" t="s">
+        <v>90</v>
+      </c>
+      <c r="F4" s="34" t="s">
         <v>455</v>
       </c>
-      <c r="G4" s="32" t="s">
+      <c r="G4" s="33" t="s">
         <v>459</v>
       </c>
-      <c r="H4" s="33"/>
-      <c r="I4" s="33"/>
-      <c r="J4" s="33"/>
-      <c r="K4" s="62"/>
-      <c r="L4" s="36" t="s">
+      <c r="H4" s="34"/>
+      <c r="I4" s="34"/>
+      <c r="J4" s="34"/>
+      <c r="K4" s="37"/>
+      <c r="L4" s="37" t="s">
         <v>460</v>
       </c>
-      <c r="M4" s="63" t="s">
+      <c r="M4" s="60" t="s">
         <v>461</v>
       </c>
       <c r="N4" s="61"/>
     </row>
     <row r="5" ht="15.75" customHeight="1">
-      <c r="A5" s="32" t="s">
+      <c r="A5" s="33" t="s">
         <v>462</v>
       </c>
-      <c r="B5" s="33" t="s">
+      <c r="B5" s="34" t="s">
         <v>463</v>
       </c>
       <c r="C5" s="20" t="s">
         <v>454</v>
       </c>
-      <c r="D5" s="33"/>
+      <c r="D5" s="34"/>
       <c r="E5" s="59" t="s">
-        <v>89</v>
-      </c>
-      <c r="F5" s="33" t="s">
+        <v>90</v>
+      </c>
+      <c r="F5" s="34" t="s">
         <v>455</v>
       </c>
-      <c r="G5" s="32" t="s">
+      <c r="G5" s="33" t="s">
         <v>464</v>
       </c>
-      <c r="H5" s="33"/>
-      <c r="I5" s="33"/>
-      <c r="J5" s="33"/>
-      <c r="K5" s="62"/>
-      <c r="L5" s="36" t="s">
+      <c r="H5" s="34"/>
+      <c r="I5" s="34"/>
+      <c r="J5" s="34"/>
+      <c r="K5" s="37"/>
+      <c r="L5" s="37" t="s">
         <v>460</v>
       </c>
-      <c r="M5" s="63" t="s">
+      <c r="M5" s="60" t="s">
         <v>465</v>
       </c>
       <c r="N5" s="61"/>
@@ -13152,53 +13153,53 @@
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
-      <c r="A1" s="64" t="s">
+      <c r="A1" s="62" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="64" t="s">
+      <c r="B1" s="62" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="64" t="s">
+      <c r="C1" s="62" t="s">
         <v>440</v>
       </c>
-      <c r="D1" s="64" t="s">
+      <c r="D1" s="62" t="s">
         <v>497</v>
       </c>
-      <c r="E1" s="64" t="s">
+      <c r="E1" s="62" t="s">
         <v>498</v>
       </c>
-      <c r="F1" s="65" t="s">
+      <c r="F1" s="62" t="s">
         <v>499</v>
       </c>
-      <c r="G1" s="65" t="s">
-        <v>436</v>
-      </c>
-      <c r="H1" s="65" t="s">
+      <c r="G1" s="63" t="s">
+        <v>500</v>
+      </c>
+      <c r="H1" s="62" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" ht="120.75" customHeight="1">
-      <c r="A2" s="65" t="s">
-        <v>500</v>
-      </c>
-      <c r="B2" s="65" t="s">
+      <c r="A2" s="64" t="s">
         <v>501</v>
       </c>
-      <c r="C2" s="65"/>
-      <c r="D2" s="66" t="s">
+      <c r="B2" s="64" t="s">
+        <v>502</v>
+      </c>
+      <c r="C2" s="64"/>
+      <c r="D2" s="65" t="s">
         <v>437</v>
       </c>
-      <c r="E2" s="67" t="s">
-        <v>502</v>
-      </c>
-      <c r="F2" s="65" t="s">
+      <c r="E2" s="66" t="s">
         <v>503</v>
       </c>
-      <c r="G2" s="65" t="s">
+      <c r="F2" s="64" t="s">
         <v>504</v>
       </c>
-      <c r="H2" s="65" t="s">
+      <c r="G2" s="64" t="s">
         <v>505</v>
+      </c>
+      <c r="H2" s="64" t="s">
+        <v>506</v>
       </c>
     </row>
   </sheetData>
@@ -13222,129 +13223,129 @@
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
-      <c r="A1" s="68" t="s">
+      <c r="A1" s="67" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" s="69" t="s">
-        <v>508</v>
-      </c>
-      <c r="C2" s="70" t="s">
+      <c r="A2" s="68" t="s">
         <v>509</v>
       </c>
+      <c r="C2" s="69" t="s">
+        <v>510</v>
+      </c>
     </row>
     <row r="3" ht="15.75" customHeight="1">
-      <c r="A3" s="71" t="s">
-        <v>510</v>
-      </c>
-      <c r="C3" s="70" t="s">
+      <c r="A3" s="70" t="s">
         <v>511</v>
       </c>
+      <c r="C3" s="69" t="s">
+        <v>512</v>
+      </c>
     </row>
     <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" s="72" t="s">
-        <v>512</v>
-      </c>
-      <c r="C4" s="70" t="s">
+      <c r="A4" s="71" t="s">
         <v>513</v>
       </c>
+      <c r="C4" s="69" t="s">
+        <v>514</v>
+      </c>
     </row>
     <row r="5" ht="15.75" customHeight="1">
-      <c r="A5" s="72" t="s">
-        <v>514</v>
-      </c>
-      <c r="C5" s="70" t="s">
+      <c r="A5" s="71" t="s">
         <v>515</v>
       </c>
+      <c r="C5" s="69" t="s">
+        <v>516</v>
+      </c>
     </row>
     <row r="6" ht="15.75" customHeight="1">
-      <c r="A6" s="69" t="s">
-        <v>516</v>
-      </c>
-      <c r="C6" s="70" t="s">
+      <c r="A6" s="68" t="s">
         <v>517</v>
       </c>
+      <c r="C6" s="69" t="s">
+        <v>518</v>
+      </c>
     </row>
     <row r="7" ht="15.75" customHeight="1">
-      <c r="A7" s="69" t="s">
-        <v>518</v>
-      </c>
-      <c r="C7" s="70" t="s">
+      <c r="A7" s="68" t="s">
         <v>519</v>
       </c>
+      <c r="C7" s="69" t="s">
+        <v>520</v>
+      </c>
     </row>
     <row r="8" ht="15.75" customHeight="1">
-      <c r="A8" s="69" t="s">
-        <v>520</v>
-      </c>
-      <c r="C8" s="70" t="s">
+      <c r="A8" s="68" t="s">
         <v>521</v>
       </c>
+      <c r="C8" s="69" t="s">
+        <v>522</v>
+      </c>
     </row>
     <row r="9" ht="15.75" customHeight="1">
-      <c r="A9" s="69" t="s">
-        <v>522</v>
-      </c>
-      <c r="C9" s="70" t="s">
+      <c r="A9" s="68" t="s">
         <v>523</v>
       </c>
+      <c r="C9" s="69" t="s">
+        <v>524</v>
+      </c>
     </row>
     <row r="10" ht="15.75" customHeight="1">
-      <c r="A10" s="69" t="s">
-        <v>524</v>
-      </c>
-      <c r="C10" s="70" t="s">
+      <c r="A10" s="68" t="s">
         <v>525</v>
       </c>
+      <c r="C10" s="69" t="s">
+        <v>526</v>
+      </c>
     </row>
     <row r="11" ht="15.75" customHeight="1">
-      <c r="A11" s="69" t="s">
-        <v>526</v>
-      </c>
-      <c r="C11" s="70" t="s">
+      <c r="A11" s="68" t="s">
         <v>527</v>
       </c>
+      <c r="C11" s="69" t="s">
+        <v>528</v>
+      </c>
     </row>
     <row r="12" ht="15.75" customHeight="1">
-      <c r="A12" s="69" t="s">
-        <v>528</v>
-      </c>
-      <c r="C12" s="70" t="s">
+      <c r="A12" s="68" t="s">
         <v>529</v>
       </c>
+      <c r="C12" s="69" t="s">
+        <v>530</v>
+      </c>
     </row>
     <row r="13" ht="15.75" customHeight="1">
-      <c r="A13" s="69" t="s">
-        <v>530</v>
-      </c>
-      <c r="C13" s="70" t="s">
+      <c r="A13" s="68" t="s">
         <v>531</v>
       </c>
+      <c r="C13" s="69" t="s">
+        <v>532</v>
+      </c>
     </row>
     <row r="14" ht="15.75" customHeight="1">
-      <c r="A14" s="69" t="s">
-        <v>532</v>
-      </c>
-      <c r="C14" s="70" t="s">
+      <c r="A14" s="68" t="s">
         <v>533</v>
       </c>
+      <c r="C14" s="69" t="s">
+        <v>534</v>
+      </c>
     </row>
     <row r="15" ht="15.75" customHeight="1">
-      <c r="A15" s="69" t="s">
-        <v>534</v>
-      </c>
-      <c r="C15" s="70" t="s">
+      <c r="A15" s="68" t="s">
         <v>535</v>
+      </c>
+      <c r="C15" s="69" t="s">
+        <v>536</v>
       </c>
     </row>
     <row r="16" ht="15.75" customHeight="1"/>

</xml_diff>